<commit_message>
reposition corsor to top left
</commit_message>
<xml_diff>
--- a/backend/fms_core/static/submission_templates/Library_QC_v4_8_0.xlsx
+++ b/backend/fms_core/static/submission_templates/Library_QC_v4_8_0.xlsx
@@ -8,9 +8,9 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="LibraryQC" sheetId="1" state="visible" r:id="rId3"/>
-    <sheet name="Info" sheetId="2" state="visible" r:id="rId4"/>
-    <sheet name="Index" sheetId="3" state="visible" r:id="rId5"/>
+    <sheet name="LibraryQC" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Info" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Index" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName function="false" hidden="false" name="Double_stranded" vbProcedure="false">Index!$H$2</definedName>
@@ -28,16 +28,18 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
-    <author>Unknown Author</author>
+    <author> </author>
   </authors>
   <commentList>
     <comment ref="E5" authorId="0">
       <text>
         <r>
           <rPr>
-            <sz val="10"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
             <rFont val="Arial"/>
-            <family val="2"/>
+            <family val="0"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Volume measured before removing Volume used</t>
         </r>
@@ -1434,7 +1436,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1508,11 +1510,6 @@
       <name val="Calibri"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -1869,6 +1866,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1877,15 +1878,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1969,114 +1966,8 @@
 </styleSheet>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
-  <a:themeElements>
-    <a:clrScheme name="LibreOffice">
-      <a:dk1>
-        <a:srgbClr val="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:srgbClr val="ffffff"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="000000"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="ffffff"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="18a303"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="0369a3"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="a33e03"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="8e03a3"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="c99c00"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="c9211e"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0000ee"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="551a8b"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
-        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
-        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme>
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-          <a:miter/>
-        </a:ln>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-          <a:miter/>
-        </a:ln>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-          <a:miter/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-</a:theme>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -2085,10 +1976,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
+      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.55859375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.55078125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="25.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="27.88"/>
@@ -25142,7 +25033,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -25152,7 +25043,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.4765625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.46875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="47.19"/>
   </cols>
@@ -26861,7 +26752,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -26871,7 +26762,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.55859375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.55078125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="9.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="16.5"/>

</xml_diff>

<commit_message>
Minor changes to format.
</commit_message>
<xml_diff>
--- a/backend/fms_core/static/submission_templates/Library_QC_v4_8_0.xlsx
+++ b/backend/fms_core/static/submission_templates/Library_QC_v4_8_0.xlsx
@@ -8,9 +8,9 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="LibraryQC" sheetId="1" state="visible" r:id="rId3"/>
-    <sheet name="Info" sheetId="2" state="visible" r:id="rId4"/>
-    <sheet name="Index" sheetId="3" state="visible" r:id="rId5"/>
+    <sheet name="LibraryQC" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Info" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Index" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName function="false" hidden="false" name="Double_stranded" vbProcedure="false">Index!$H$2</definedName>
@@ -28,7 +28,7 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
-    <author>Unknown Author</author>
+    <author>UFG</author>
   </authors>
   <commentList>
     <comment ref="E5" authorId="0">
@@ -38,6 +38,7 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Volume measured before removing Volume used</t>
         </r>
@@ -1435,7 +1436,7 @@
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="General"/>
   </numFmts>
-  <fonts count="17">
+  <fonts count="16">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1505,15 +1506,9 @@
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
     </font>
     <font>
       <i val="true"/>
@@ -1527,6 +1522,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -1730,7 +1726,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="48">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1819,7 +1815,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1843,11 +1839,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="12" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1859,7 +1855,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1883,11 +1879,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1899,15 +1903,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1991,114 +1991,8 @@
 </styleSheet>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
-  <a:themeElements>
-    <a:clrScheme name="LibreOffice">
-      <a:dk1>
-        <a:srgbClr val="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:srgbClr val="ffffff"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="000000"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="ffffff"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="18a303"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="0369a3"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="a33e03"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="8e03a3"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="c99c00"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="c9211e"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0000ee"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="551a8b"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
-        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
-        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme>
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-          <a:miter/>
-        </a:ln>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-          <a:miter/>
-        </a:ln>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-          <a:miter/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-</a:theme>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -2110,7 +2004,7 @@
       <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.55859375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.55078125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="25.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="27.88"/>
@@ -25112,7 +25006,7 @@
       <c r="H1000" s="36"/>
       <c r="I1000" s="36"/>
       <c r="J1000" s="36"/>
-      <c r="K1000" s="18" t="str">
+      <c r="K1000" s="38" t="str">
         <f aca="true">IF(OR(AND(ISBLANK(D1000), ISBLANK(E1000)),AND(OR(ISBLANK(G1000),ISBLANK(H1000),ISBLANK(I1000)),ISBLANK(J1000))),"",IF(ISBLANK(J1000),IF(ISBLANK(E1000),(D1000-F1000)*I1000*H1000*INDIRECT(SUBSTITUTE(G1000," ","_"))/1000000,(E1000-F1000)*I1000*H1000*INDIRECT(SUBSTITUTE(G1000," ","_"))/1000000),IF(ISBLANK(E1000),(D1000-F1000)*J1000,(E1000-F1000)*J1000)))</f>
         <v/>
       </c>
@@ -25120,36 +25014,36 @@
       <c r="M1000" s="37"/>
       <c r="N1000" s="37"/>
       <c r="O1000" s="34"/>
-      <c r="P1000" s="38"/>
-      <c r="Q1000" s="38"/>
-      <c r="R1000" s="39"/>
+      <c r="P1000" s="39"/>
+      <c r="Q1000" s="39"/>
+      <c r="R1000" s="40"/>
     </row>
   </sheetData>
   <dataValidations count="5">
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G6:G1000" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G6:G1000" type="list">
       <formula1>Index!$F$2:$F$3</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="M6:M1000 O6:O1000" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="M6:M1000 O6:O1000" type="list">
       <formula1>Index!$C$2:$C$3</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="R6:R1000" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="R6:R1000" type="list">
       <formula1>Index!$K$2:$K$5</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="L6:L1000" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="L6:L1000" type="list">
       <formula1>Index!$D$2:$D$3</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="N6:N1000" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="N6:N1000" type="list">
       <formula1>Index!$E$2:$E$3</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -25159,7 +25053,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -25169,13 +25063,13 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.4765625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.46875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="47.19"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="41" t="s">
         <v>22</v>
       </c>
       <c r="B1" s="3"/>
@@ -25367,7 +25261,7 @@
       <c r="X7" s="3"/>
     </row>
     <row r="8" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="41" t="s">
+      <c r="A8" s="42" t="s">
         <v>27</v>
       </c>
       <c r="D8" s="3"/>
@@ -25393,7 +25287,7 @@
       <c r="X8" s="3"/>
     </row>
     <row r="9" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="42"/>
+      <c r="B9" s="43"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
@@ -25417,13 +25311,13 @@
       <c r="X9" s="3"/>
     </row>
     <row r="10" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="43" t="s">
+      <c r="A10" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="44" t="s">
+      <c r="B10" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="45"/>
+      <c r="C10" s="46"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
@@ -25447,13 +25341,13 @@
       <c r="X10" s="3"/>
     </row>
     <row r="11" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="43" t="s">
+      <c r="A11" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="44" t="s">
+      <c r="B11" s="45" t="s">
         <v>29</v>
       </c>
-      <c r="C11" s="45"/>
+      <c r="C11" s="46"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
@@ -25477,13 +25371,13 @@
       <c r="X11" s="3"/>
     </row>
     <row r="12" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="43" t="s">
+      <c r="A12" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="44" t="s">
+      <c r="B12" s="45" t="s">
         <v>30</v>
       </c>
-      <c r="C12" s="45"/>
+      <c r="C12" s="46"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
@@ -25507,13 +25401,13 @@
       <c r="X12" s="3"/>
     </row>
     <row r="13" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="43" t="s">
+      <c r="A13" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="44" t="s">
+      <c r="B13" s="45" t="s">
         <v>31</v>
       </c>
-      <c r="C13" s="45"/>
+      <c r="C13" s="46"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
@@ -25537,13 +25431,13 @@
       <c r="X13" s="3"/>
     </row>
     <row r="14" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="43" t="s">
+      <c r="A14" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="44" t="s">
+      <c r="B14" s="45" t="s">
         <v>32</v>
       </c>
-      <c r="C14" s="45"/>
+      <c r="C14" s="46"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
@@ -25567,13 +25461,13 @@
       <c r="X14" s="3"/>
     </row>
     <row r="15" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="43" t="s">
+      <c r="A15" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="44" t="s">
+      <c r="B15" s="45" t="s">
         <v>33</v>
       </c>
-      <c r="C15" s="45"/>
+      <c r="C15" s="46"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
@@ -25597,13 +25491,13 @@
       <c r="X15" s="3"/>
     </row>
     <row r="16" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="43" t="s">
+      <c r="A16" s="44" t="s">
         <v>10</v>
       </c>
-      <c r="B16" s="44" t="s">
+      <c r="B16" s="45" t="s">
         <v>34</v>
       </c>
-      <c r="C16" s="45"/>
+      <c r="C16" s="46"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
@@ -25627,13 +25521,13 @@
       <c r="X16" s="3"/>
     </row>
     <row r="17" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="43" t="s">
+      <c r="A17" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="B17" s="44" t="s">
+      <c r="B17" s="45" t="s">
         <v>35</v>
       </c>
-      <c r="C17" s="45"/>
+      <c r="C17" s="46"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
@@ -25657,13 +25551,13 @@
       <c r="X17" s="3"/>
     </row>
     <row r="18" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="43" t="s">
+      <c r="A18" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="B18" s="44" t="s">
+      <c r="B18" s="45" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="45"/>
+      <c r="C18" s="46"/>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
@@ -25687,13 +25581,13 @@
       <c r="X18" s="3"/>
     </row>
     <row r="19" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="43" t="s">
+      <c r="A19" s="44" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="44" t="s">
+      <c r="B19" s="45" t="s">
         <v>37</v>
       </c>
-      <c r="C19" s="45"/>
+      <c r="C19" s="46"/>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
@@ -25717,13 +25611,13 @@
       <c r="X19" s="3"/>
     </row>
     <row r="20" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="43" t="s">
+      <c r="A20" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="44" t="s">
+      <c r="B20" s="45" t="s">
         <v>38</v>
       </c>
-      <c r="C20" s="45"/>
+      <c r="C20" s="46"/>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
@@ -25747,13 +25641,13 @@
       <c r="X20" s="3"/>
     </row>
     <row r="21" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="43" t="s">
+      <c r="A21" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="B21" s="44" t="s">
+      <c r="B21" s="45" t="s">
         <v>39</v>
       </c>
-      <c r="C21" s="45"/>
+      <c r="C21" s="46"/>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
@@ -25777,13 +25671,13 @@
       <c r="X21" s="3"/>
     </row>
     <row r="22" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="43" t="s">
+      <c r="A22" s="44" t="s">
         <v>16</v>
       </c>
-      <c r="B22" s="44" t="s">
+      <c r="B22" s="45" t="s">
         <v>40</v>
       </c>
-      <c r="C22" s="45"/>
+      <c r="C22" s="46"/>
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
@@ -25807,13 +25701,13 @@
       <c r="X22" s="3"/>
     </row>
     <row r="23" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="43" t="s">
+      <c r="A23" s="44" t="s">
         <v>17</v>
       </c>
-      <c r="B23" s="44" t="s">
+      <c r="B23" s="45" t="s">
         <v>41</v>
       </c>
-      <c r="C23" s="45"/>
+      <c r="C23" s="46"/>
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
@@ -25837,13 +25731,13 @@
       <c r="X23" s="3"/>
     </row>
     <row r="24" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="43" t="s">
+      <c r="A24" s="44" t="s">
         <v>18</v>
       </c>
-      <c r="B24" s="44" t="s">
+      <c r="B24" s="45" t="s">
         <v>42</v>
       </c>
-      <c r="C24" s="45"/>
+      <c r="C24" s="46"/>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
@@ -25867,13 +25761,13 @@
       <c r="X24" s="3"/>
     </row>
     <row r="25" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="43" t="s">
+      <c r="A25" s="44" t="s">
         <v>19</v>
       </c>
-      <c r="B25" s="44" t="s">
+      <c r="B25" s="45" t="s">
         <v>43</v>
       </c>
-      <c r="C25" s="45"/>
+      <c r="C25" s="46"/>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
@@ -25897,13 +25791,13 @@
       <c r="X25" s="3"/>
     </row>
     <row r="26" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="43" t="s">
+      <c r="A26" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="B26" s="44" t="s">
+      <c r="B26" s="45" t="s">
         <v>44</v>
       </c>
-      <c r="C26" s="45"/>
+      <c r="C26" s="46"/>
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
@@ -25927,13 +25821,13 @@
       <c r="X26" s="3"/>
     </row>
     <row r="27" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="43" t="s">
+      <c r="A27" s="44" t="s">
         <v>21</v>
       </c>
-      <c r="B27" s="44" t="s">
+      <c r="B27" s="45" t="s">
         <v>45</v>
       </c>
-      <c r="C27" s="45"/>
+      <c r="C27" s="46"/>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
       <c r="F27" s="3"/>
@@ -26869,7 +26763,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -26878,7 +26772,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -26888,7 +26782,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.55859375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.55078125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="9.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="16.5"/>
@@ -26901,2340 +26795,2340 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="47" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="47" t="s">
         <v>47</v>
       </c>
-      <c r="C1" s="46" t="s">
+      <c r="C1" s="47" t="s">
         <v>48</v>
       </c>
-      <c r="D1" s="46" t="s">
+      <c r="D1" s="47" t="s">
         <v>49</v>
       </c>
-      <c r="E1" s="46" t="s">
+      <c r="E1" s="47" t="s">
         <v>50</v>
       </c>
-      <c r="F1" s="46" t="s">
+      <c r="F1" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46" t="s">
+      <c r="G1" s="47"/>
+      <c r="H1" s="47" t="s">
         <v>51</v>
       </c>
-      <c r="I1" s="46" t="s">
+      <c r="I1" s="47" t="s">
         <v>52</v>
       </c>
-      <c r="J1" s="46"/>
-      <c r="K1" s="46" t="s">
+      <c r="J1" s="47"/>
+      <c r="K1" s="47" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="46" t="s">
+      <c r="A2" s="47" t="s">
         <v>53</v>
       </c>
-      <c r="B2" s="46" t="s">
+      <c r="B2" s="47" t="s">
         <v>53</v>
       </c>
-      <c r="C2" s="46" t="s">
+      <c r="C2" s="47" t="s">
         <v>54</v>
       </c>
-      <c r="D2" s="46" t="s">
+      <c r="D2" s="47" t="s">
         <v>55</v>
       </c>
-      <c r="E2" s="46" t="s">
+      <c r="E2" s="47" t="s">
         <v>56</v>
       </c>
-      <c r="F2" s="46" t="s">
+      <c r="F2" s="47" t="s">
         <v>57</v>
       </c>
-      <c r="G2" s="46"/>
-      <c r="H2" s="46" t="n">
+      <c r="G2" s="47"/>
+      <c r="H2" s="47" t="n">
         <v>617.9</v>
       </c>
-      <c r="I2" s="46" t="n">
+      <c r="I2" s="47" t="n">
         <f aca="false">H2/2</f>
         <v>308.95</v>
       </c>
-      <c r="J2" s="46"/>
-      <c r="K2" s="46" t="s">
+      <c r="J2" s="47"/>
+      <c r="K2" s="47" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="46" t="s">
+      <c r="A3" s="47" t="s">
         <v>59</v>
       </c>
-      <c r="B3" s="46" t="s">
+      <c r="B3" s="47" t="s">
         <v>59</v>
       </c>
-      <c r="C3" s="46" t="s">
+      <c r="C3" s="47" t="s">
         <v>60</v>
       </c>
-      <c r="D3" s="46" t="s">
+      <c r="D3" s="47" t="s">
         <v>61</v>
       </c>
-      <c r="E3" s="46" t="s">
+      <c r="E3" s="47" t="s">
         <v>62</v>
       </c>
-      <c r="F3" s="46" t="s">
+      <c r="F3" s="47" t="s">
         <v>63</v>
       </c>
-      <c r="G3" s="46"/>
-      <c r="H3" s="46"/>
-      <c r="I3" s="46"/>
-      <c r="J3" s="46"/>
-      <c r="K3" s="46" t="s">
+      <c r="G3" s="47"/>
+      <c r="H3" s="47"/>
+      <c r="I3" s="47"/>
+      <c r="J3" s="47"/>
+      <c r="K3" s="47" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="46" t="s">
+      <c r="A4" s="47" t="s">
         <v>65</v>
       </c>
-      <c r="B4" s="46" t="s">
+      <c r="B4" s="47" t="s">
         <v>65</v>
       </c>
-      <c r="C4" s="46"/>
-      <c r="D4" s="46"/>
-      <c r="E4" s="46"/>
-      <c r="F4" s="46"/>
-      <c r="G4" s="46"/>
-      <c r="H4" s="46"/>
-      <c r="I4" s="46"/>
-      <c r="J4" s="46"/>
-      <c r="K4" s="46" t="s">
+      <c r="C4" s="47"/>
+      <c r="D4" s="47"/>
+      <c r="E4" s="47"/>
+      <c r="F4" s="47"/>
+      <c r="G4" s="47"/>
+      <c r="H4" s="47"/>
+      <c r="I4" s="47"/>
+      <c r="J4" s="47"/>
+      <c r="K4" s="47" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="46" t="s">
+      <c r="A5" s="47" t="s">
         <v>67</v>
       </c>
-      <c r="B5" s="46" t="s">
+      <c r="B5" s="47" t="s">
         <v>67</v>
       </c>
-      <c r="C5" s="46"/>
-      <c r="E5" s="46"/>
-      <c r="F5" s="46"/>
-      <c r="G5" s="46"/>
-      <c r="H5" s="46"/>
-      <c r="I5" s="46"/>
-      <c r="J5" s="46"/>
-      <c r="K5" s="46" t="s">
+      <c r="C5" s="47"/>
+      <c r="E5" s="47"/>
+      <c r="F5" s="47"/>
+      <c r="G5" s="47"/>
+      <c r="H5" s="47"/>
+      <c r="I5" s="47"/>
+      <c r="J5" s="47"/>
+      <c r="K5" s="47" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="46" t="s">
+      <c r="A6" s="47" t="s">
         <v>69</v>
       </c>
-      <c r="B6" s="46" t="s">
+      <c r="B6" s="47" t="s">
         <v>69</v>
       </c>
-      <c r="C6" s="46"/>
-      <c r="D6" s="46"/>
-      <c r="E6" s="46"/>
-      <c r="F6" s="46"/>
-      <c r="G6" s="46"/>
-      <c r="H6" s="46"/>
-      <c r="I6" s="46"/>
-      <c r="J6" s="46"/>
-      <c r="K6" s="46"/>
+      <c r="C6" s="47"/>
+      <c r="D6" s="47"/>
+      <c r="E6" s="47"/>
+      <c r="F6" s="47"/>
+      <c r="G6" s="47"/>
+      <c r="H6" s="47"/>
+      <c r="I6" s="47"/>
+      <c r="J6" s="47"/>
+      <c r="K6" s="47"/>
     </row>
     <row r="7" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="46" t="s">
+      <c r="A7" s="47" t="s">
         <v>70</v>
       </c>
-      <c r="B7" s="46" t="s">
+      <c r="B7" s="47" t="s">
         <v>70</v>
       </c>
-      <c r="C7" s="46"/>
-      <c r="D7" s="46"/>
-      <c r="E7" s="46"/>
-      <c r="F7" s="46"/>
-      <c r="G7" s="46"/>
-      <c r="H7" s="46"/>
-      <c r="I7" s="46"/>
-      <c r="J7" s="46"/>
-      <c r="K7" s="46"/>
+      <c r="C7" s="47"/>
+      <c r="D7" s="47"/>
+      <c r="E7" s="47"/>
+      <c r="F7" s="47"/>
+      <c r="G7" s="47"/>
+      <c r="H7" s="47"/>
+      <c r="I7" s="47"/>
+      <c r="J7" s="47"/>
+      <c r="K7" s="47"/>
     </row>
     <row r="8" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="46" t="s">
+      <c r="A8" s="47" t="s">
         <v>71</v>
       </c>
-      <c r="B8" s="46" t="s">
+      <c r="B8" s="47" t="s">
         <v>71</v>
       </c>
-      <c r="C8" s="46"/>
-      <c r="D8" s="46"/>
-      <c r="E8" s="46"/>
-      <c r="F8" s="46"/>
-      <c r="G8" s="46"/>
-      <c r="H8" s="46"/>
-      <c r="I8" s="46"/>
-      <c r="J8" s="46"/>
-      <c r="K8" s="46"/>
+      <c r="C8" s="47"/>
+      <c r="D8" s="47"/>
+      <c r="E8" s="47"/>
+      <c r="F8" s="47"/>
+      <c r="G8" s="47"/>
+      <c r="H8" s="47"/>
+      <c r="I8" s="47"/>
+      <c r="J8" s="47"/>
+      <c r="K8" s="47"/>
     </row>
     <row r="9" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="46" t="s">
+      <c r="A9" s="47" t="s">
         <v>72</v>
       </c>
-      <c r="B9" s="46" t="s">
+      <c r="B9" s="47" t="s">
         <v>72</v>
       </c>
-      <c r="C9" s="46"/>
-      <c r="E9" s="46"/>
-      <c r="K9" s="46"/>
+      <c r="C9" s="47"/>
+      <c r="E9" s="47"/>
+      <c r="K9" s="47"/>
     </row>
     <row r="10" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="46" t="s">
+      <c r="A10" s="47" t="s">
         <v>73</v>
       </c>
-      <c r="B10" s="46" t="s">
+      <c r="B10" s="47" t="s">
         <v>73</v>
       </c>
-      <c r="C10" s="46"/>
+      <c r="C10" s="47"/>
     </row>
     <row r="11" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="46" t="s">
+      <c r="A11" s="47" t="s">
         <v>74</v>
       </c>
-      <c r="B11" s="46" t="s">
+      <c r="B11" s="47" t="s">
         <v>74</v>
       </c>
-      <c r="C11" s="46"/>
+      <c r="C11" s="47"/>
     </row>
     <row r="12" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="46" t="s">
+      <c r="A12" s="47" t="s">
         <v>75</v>
       </c>
-      <c r="B12" s="46" t="s">
+      <c r="B12" s="47" t="s">
         <v>75</v>
       </c>
-      <c r="C12" s="46"/>
+      <c r="C12" s="47"/>
     </row>
     <row r="13" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="46" t="s">
+      <c r="A13" s="47" t="s">
         <v>76</v>
       </c>
-      <c r="B13" s="46" t="s">
+      <c r="B13" s="47" t="s">
         <v>76</v>
       </c>
-      <c r="C13" s="46"/>
+      <c r="C13" s="47"/>
     </row>
     <row r="14" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="46" t="s">
+      <c r="A14" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="B14" s="46" t="s">
+      <c r="B14" s="47" t="s">
         <v>78</v>
       </c>
-      <c r="C14" s="46"/>
+      <c r="C14" s="47"/>
     </row>
     <row r="15" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="46" t="s">
+      <c r="A15" s="47" t="s">
         <v>79</v>
       </c>
-      <c r="B15" s="46" t="s">
+      <c r="B15" s="47" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="46" t="s">
+      <c r="A16" s="47" t="s">
         <v>81</v>
       </c>
-      <c r="B16" s="46" t="s">
+      <c r="B16" s="47" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="46" t="s">
+      <c r="A17" s="47" t="s">
         <v>83</v>
       </c>
-      <c r="B17" s="46" t="s">
+      <c r="B17" s="47" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="46" t="s">
+      <c r="A18" s="47" t="s">
         <v>85</v>
       </c>
-      <c r="B18" s="46" t="s">
+      <c r="B18" s="47" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="46" t="s">
+      <c r="A19" s="47" t="s">
         <v>87</v>
       </c>
-      <c r="B19" s="46" t="s">
+      <c r="B19" s="47" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="46" t="s">
+      <c r="A20" s="47" t="s">
         <v>89</v>
       </c>
-      <c r="B20" s="46" t="s">
+      <c r="B20" s="47" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="46" t="s">
+      <c r="A21" s="47" t="s">
         <v>91</v>
       </c>
-      <c r="B21" s="46" t="s">
+      <c r="B21" s="47" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="46" t="s">
+      <c r="A22" s="47" t="s">
         <v>93</v>
       </c>
-      <c r="B22" s="46" t="s">
+      <c r="B22" s="47" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="46" t="s">
+      <c r="A23" s="47" t="s">
         <v>95</v>
       </c>
-      <c r="B23" s="46" t="s">
+      <c r="B23" s="47" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="46" t="s">
+      <c r="A24" s="47" t="s">
         <v>97</v>
       </c>
-      <c r="B24" s="46" t="s">
+      <c r="B24" s="47" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="46" t="s">
+      <c r="A25" s="47" t="s">
         <v>99</v>
       </c>
-      <c r="B25" s="46" t="s">
+      <c r="B25" s="47" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="46" t="s">
+      <c r="A26" s="47" t="s">
         <v>101</v>
       </c>
-      <c r="B26" s="46" t="s">
+      <c r="B26" s="47" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="46" t="s">
+      <c r="A27" s="47" t="s">
         <v>102</v>
       </c>
-      <c r="B27" s="46" t="s">
+      <c r="B27" s="47" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="46" t="s">
+      <c r="A28" s="47" t="s">
         <v>103</v>
       </c>
-      <c r="B28" s="46" t="s">
+      <c r="B28" s="47" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="46" t="s">
+      <c r="A29" s="47" t="s">
         <v>104</v>
       </c>
-      <c r="B29" s="46" t="s">
+      <c r="B29" s="47" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="46" t="s">
+      <c r="A30" s="47" t="s">
         <v>105</v>
       </c>
-      <c r="B30" s="46" t="s">
+      <c r="B30" s="47" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="46" t="s">
+      <c r="A31" s="47" t="s">
         <v>106</v>
       </c>
-      <c r="B31" s="46" t="s">
+      <c r="B31" s="47" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="46" t="s">
+      <c r="A32" s="47" t="s">
         <v>107</v>
       </c>
-      <c r="B32" s="46" t="s">
+      <c r="B32" s="47" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="46" t="s">
+      <c r="A33" s="47" t="s">
         <v>108</v>
       </c>
-      <c r="B33" s="46" t="s">
+      <c r="B33" s="47" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="46" t="s">
+      <c r="A34" s="47" t="s">
         <v>109</v>
       </c>
-      <c r="B34" s="46" t="s">
+      <c r="B34" s="47" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="46" t="s">
+      <c r="A35" s="47" t="s">
         <v>110</v>
       </c>
-      <c r="B35" s="46" t="s">
+      <c r="B35" s="47" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="46" t="s">
+      <c r="A36" s="47" t="s">
         <v>111</v>
       </c>
-      <c r="B36" s="46" t="s">
+      <c r="B36" s="47" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="46" t="s">
+      <c r="A37" s="47" t="s">
         <v>112</v>
       </c>
-      <c r="B37" s="46" t="s">
+      <c r="B37" s="47" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="46" t="s">
+      <c r="A38" s="47" t="s">
         <v>113</v>
       </c>
-      <c r="B38" s="46" t="s">
+      <c r="B38" s="47" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A39" s="46" t="s">
+      <c r="A39" s="47" t="s">
         <v>115</v>
       </c>
-      <c r="B39" s="46" t="s">
+      <c r="B39" s="47" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A40" s="46" t="s">
+      <c r="A40" s="47" t="s">
         <v>117</v>
       </c>
-      <c r="B40" s="46" t="s">
+      <c r="B40" s="47" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A41" s="46" t="s">
+      <c r="A41" s="47" t="s">
         <v>119</v>
       </c>
-      <c r="B41" s="46" t="s">
+      <c r="B41" s="47" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A42" s="46" t="s">
+      <c r="A42" s="47" t="s">
         <v>121</v>
       </c>
-      <c r="B42" s="46" t="s">
+      <c r="B42" s="47" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A43" s="46" t="s">
+      <c r="A43" s="47" t="s">
         <v>123</v>
       </c>
-      <c r="B43" s="46" t="s">
+      <c r="B43" s="47" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A44" s="46" t="s">
+      <c r="A44" s="47" t="s">
         <v>125</v>
       </c>
-      <c r="B44" s="46" t="s">
+      <c r="B44" s="47" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A45" s="46" t="s">
+      <c r="A45" s="47" t="s">
         <v>127</v>
       </c>
-      <c r="B45" s="46" t="s">
+      <c r="B45" s="47" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A46" s="46" t="s">
+      <c r="A46" s="47" t="s">
         <v>129</v>
       </c>
-      <c r="B46" s="46" t="s">
+      <c r="B46" s="47" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A47" s="46" t="s">
+      <c r="A47" s="47" t="s">
         <v>131</v>
       </c>
-      <c r="B47" s="46" t="s">
+      <c r="B47" s="47" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A48" s="46" t="s">
+      <c r="A48" s="47" t="s">
         <v>133</v>
       </c>
-      <c r="B48" s="46" t="s">
+      <c r="B48" s="47" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A49" s="46" t="s">
+      <c r="A49" s="47" t="s">
         <v>135</v>
       </c>
-      <c r="B49" s="46" t="s">
+      <c r="B49" s="47" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A50" s="46" t="s">
+      <c r="A50" s="47" t="s">
         <v>137</v>
       </c>
-      <c r="B50" s="46" t="s">
+      <c r="B50" s="47" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A51" s="46" t="s">
+      <c r="A51" s="47" t="s">
         <v>138</v>
       </c>
-      <c r="B51" s="46" t="s">
+      <c r="B51" s="47" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A52" s="46" t="s">
+      <c r="A52" s="47" t="s">
         <v>139</v>
       </c>
-      <c r="B52" s="46" t="s">
+      <c r="B52" s="47" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A53" s="46" t="s">
+      <c r="A53" s="47" t="s">
         <v>140</v>
       </c>
-      <c r="B53" s="46" t="s">
+      <c r="B53" s="47" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A54" s="46" t="s">
+      <c r="A54" s="47" t="s">
         <v>141</v>
       </c>
-      <c r="B54" s="46" t="s">
+      <c r="B54" s="47" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A55" s="46" t="s">
+      <c r="A55" s="47" t="s">
         <v>142</v>
       </c>
-      <c r="B55" s="46" t="s">
+      <c r="B55" s="47" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A56" s="46" t="s">
+      <c r="A56" s="47" t="s">
         <v>143</v>
       </c>
-      <c r="B56" s="46" t="s">
+      <c r="B56" s="47" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A57" s="46" t="s">
+      <c r="A57" s="47" t="s">
         <v>144</v>
       </c>
-      <c r="B57" s="46" t="s">
+      <c r="B57" s="47" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A58" s="46" t="s">
+      <c r="A58" s="47" t="s">
         <v>145</v>
       </c>
-      <c r="B58" s="46" t="s">
+      <c r="B58" s="47" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A59" s="46" t="s">
+      <c r="A59" s="47" t="s">
         <v>146</v>
       </c>
-      <c r="B59" s="46" t="s">
+      <c r="B59" s="47" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A60" s="46" t="s">
+      <c r="A60" s="47" t="s">
         <v>147</v>
       </c>
-      <c r="B60" s="46" t="s">
+      <c r="B60" s="47" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A61" s="46" t="s">
+      <c r="A61" s="47" t="s">
         <v>148</v>
       </c>
-      <c r="B61" s="46" t="s">
+      <c r="B61" s="47" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A62" s="46" t="s">
+      <c r="A62" s="47" t="s">
         <v>149</v>
       </c>
-      <c r="B62" s="46" t="s">
+      <c r="B62" s="47" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A63" s="46" t="s">
+      <c r="A63" s="47" t="s">
         <v>151</v>
       </c>
-      <c r="B63" s="46" t="s">
+      <c r="B63" s="47" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A64" s="46" t="s">
+      <c r="A64" s="47" t="s">
         <v>153</v>
       </c>
-      <c r="B64" s="46" t="s">
+      <c r="B64" s="47" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A65" s="46" t="s">
+      <c r="A65" s="47" t="s">
         <v>155</v>
       </c>
-      <c r="B65" s="46" t="s">
+      <c r="B65" s="47" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A66" s="46" t="s">
+      <c r="A66" s="47" t="s">
         <v>157</v>
       </c>
-      <c r="B66" s="46" t="s">
+      <c r="B66" s="47" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A67" s="46" t="s">
+      <c r="A67" s="47" t="s">
         <v>159</v>
       </c>
-      <c r="B67" s="46" t="s">
+      <c r="B67" s="47" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A68" s="46" t="s">
+      <c r="A68" s="47" t="s">
         <v>161</v>
       </c>
-      <c r="B68" s="46" t="s">
+      <c r="B68" s="47" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A69" s="46" t="s">
+      <c r="A69" s="47" t="s">
         <v>163</v>
       </c>
-      <c r="B69" s="46" t="s">
+      <c r="B69" s="47" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A70" s="46" t="s">
+      <c r="A70" s="47" t="s">
         <v>165</v>
       </c>
-      <c r="B70" s="46" t="s">
+      <c r="B70" s="47" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A71" s="46" t="s">
+      <c r="A71" s="47" t="s">
         <v>167</v>
       </c>
-      <c r="B71" s="46" t="s">
+      <c r="B71" s="47" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A72" s="46" t="s">
+      <c r="A72" s="47" t="s">
         <v>169</v>
       </c>
-      <c r="B72" s="46" t="s">
+      <c r="B72" s="47" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A73" s="46" t="s">
+      <c r="A73" s="47" t="s">
         <v>171</v>
       </c>
-      <c r="B73" s="46" t="s">
+      <c r="B73" s="47" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A74" s="46" t="s">
+      <c r="A74" s="47" t="s">
         <v>173</v>
       </c>
-      <c r="B74" s="46" t="s">
+      <c r="B74" s="47" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A75" s="46" t="s">
+      <c r="A75" s="47" t="s">
         <v>174</v>
       </c>
-      <c r="B75" s="46" t="s">
+      <c r="B75" s="47" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A76" s="46" t="s">
+      <c r="A76" s="47" t="s">
         <v>175</v>
       </c>
-      <c r="B76" s="46" t="s">
+      <c r="B76" s="47" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A77" s="46" t="s">
+      <c r="A77" s="47" t="s">
         <v>176</v>
       </c>
-      <c r="B77" s="46" t="s">
+      <c r="B77" s="47" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A78" s="46" t="s">
+      <c r="A78" s="47" t="s">
         <v>177</v>
       </c>
-      <c r="B78" s="46" t="s">
+      <c r="B78" s="47" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A79" s="46" t="s">
+      <c r="A79" s="47" t="s">
         <v>178</v>
       </c>
-      <c r="B79" s="46" t="s">
+      <c r="B79" s="47" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A80" s="46" t="s">
+      <c r="A80" s="47" t="s">
         <v>179</v>
       </c>
-      <c r="B80" s="46" t="s">
+      <c r="B80" s="47" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A81" s="46" t="s">
+      <c r="A81" s="47" t="s">
         <v>180</v>
       </c>
-      <c r="B81" s="46" t="s">
+      <c r="B81" s="47" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A82" s="46" t="s">
+      <c r="A82" s="47" t="s">
         <v>181</v>
       </c>
-      <c r="B82" s="46" t="s">
+      <c r="B82" s="47" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A83" s="46" t="s">
+      <c r="A83" s="47" t="s">
         <v>182</v>
       </c>
-      <c r="B83" s="46" t="s">
+      <c r="B83" s="47" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A84" s="46" t="s">
+      <c r="A84" s="47" t="s">
         <v>183</v>
       </c>
-      <c r="B84" s="46" t="s">
+      <c r="B84" s="47" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A85" s="46" t="s">
+      <c r="A85" s="47" t="s">
         <v>184</v>
       </c>
-      <c r="B85" s="46" t="s">
+      <c r="B85" s="47" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A86" s="46" t="s">
+      <c r="A86" s="47" t="s">
         <v>185</v>
       </c>
-      <c r="B86" s="46" t="s">
+      <c r="B86" s="47" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A87" s="46" t="s">
+      <c r="A87" s="47" t="s">
         <v>187</v>
       </c>
-      <c r="B87" s="46" t="s">
+      <c r="B87" s="47" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A88" s="46" t="s">
+      <c r="A88" s="47" t="s">
         <v>189</v>
       </c>
-      <c r="B88" s="46" t="s">
+      <c r="B88" s="47" t="s">
         <v>190</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A89" s="46" t="s">
+      <c r="A89" s="47" t="s">
         <v>191</v>
       </c>
-      <c r="B89" s="46" t="s">
+      <c r="B89" s="47" t="s">
         <v>192</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A90" s="46" t="s">
+      <c r="A90" s="47" t="s">
         <v>193</v>
       </c>
-      <c r="B90" s="46" t="s">
+      <c r="B90" s="47" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A91" s="46" t="s">
+      <c r="A91" s="47" t="s">
         <v>195</v>
       </c>
-      <c r="B91" s="46" t="s">
+      <c r="B91" s="47" t="s">
         <v>196</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A92" s="46" t="s">
+      <c r="A92" s="47" t="s">
         <v>197</v>
       </c>
-      <c r="B92" s="46" t="s">
+      <c r="B92" s="47" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A93" s="46" t="s">
+      <c r="A93" s="47" t="s">
         <v>199</v>
       </c>
-      <c r="B93" s="46" t="s">
+      <c r="B93" s="47" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A94" s="46" t="s">
+      <c r="A94" s="47" t="s">
         <v>201</v>
       </c>
-      <c r="B94" s="46" t="s">
+      <c r="B94" s="47" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A95" s="46" t="s">
+      <c r="A95" s="47" t="s">
         <v>203</v>
       </c>
-      <c r="B95" s="46" t="s">
+      <c r="B95" s="47" t="s">
         <v>204</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A96" s="46" t="s">
+      <c r="A96" s="47" t="s">
         <v>205</v>
       </c>
-      <c r="B96" s="46" t="s">
+      <c r="B96" s="47" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A97" s="46" t="s">
+      <c r="A97" s="47" t="s">
         <v>207</v>
       </c>
-      <c r="B97" s="46" t="s">
+      <c r="B97" s="47" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B98" s="46" t="s">
+      <c r="B98" s="47" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B99" s="46" t="s">
+      <c r="B99" s="47" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B100" s="46" t="s">
+      <c r="B100" s="47" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B101" s="46" t="s">
+      <c r="B101" s="47" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B102" s="46" t="s">
+      <c r="B102" s="47" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B103" s="46" t="s">
+      <c r="B103" s="47" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B104" s="46" t="s">
+      <c r="B104" s="47" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B105" s="46" t="s">
+      <c r="B105" s="47" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B106" s="46" t="s">
+      <c r="B106" s="47" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B107" s="46" t="s">
+      <c r="B107" s="47" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B108" s="46" t="s">
+      <c r="B108" s="47" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B109" s="46" t="s">
+      <c r="B109" s="47" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B110" s="46" t="s">
+      <c r="B110" s="47" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B111" s="46" t="s">
+      <c r="B111" s="47" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B112" s="46" t="s">
+      <c r="B112" s="47" t="s">
         <v>211</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B113" s="46" t="s">
+      <c r="B113" s="47" t="s">
         <v>212</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B114" s="46" t="s">
+      <c r="B114" s="47" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B115" s="46" t="s">
+      <c r="B115" s="47" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B116" s="46" t="s">
+      <c r="B116" s="47" t="s">
         <v>215</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B117" s="46" t="s">
+      <c r="B117" s="47" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B118" s="46" t="s">
+      <c r="B118" s="47" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B119" s="46" t="s">
+      <c r="B119" s="47" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B120" s="46" t="s">
+      <c r="B120" s="47" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B121" s="46" t="s">
+      <c r="B121" s="47" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B122" s="46" t="s">
+      <c r="B122" s="47" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B123" s="46" t="s">
+      <c r="B123" s="47" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B124" s="46" t="s">
+      <c r="B124" s="47" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B125" s="46" t="s">
+      <c r="B125" s="47" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B126" s="46" t="s">
+      <c r="B126" s="47" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B127" s="46" t="s">
+      <c r="B127" s="47" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B128" s="46" t="s">
+      <c r="B128" s="47" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B129" s="46" t="s">
+      <c r="B129" s="47" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B130" s="46" t="s">
+      <c r="B130" s="47" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B131" s="46" t="s">
+      <c r="B131" s="47" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B132" s="46" t="s">
+      <c r="B132" s="47" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B133" s="46" t="s">
+      <c r="B133" s="47" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B134" s="46" t="s">
+      <c r="B134" s="47" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B135" s="46" t="s">
+      <c r="B135" s="47" t="s">
         <v>222</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B136" s="46" t="s">
+      <c r="B136" s="47" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B137" s="46" t="s">
+      <c r="B137" s="47" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B138" s="46" t="s">
+      <c r="B138" s="47" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B139" s="46" t="s">
+      <c r="B139" s="47" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B140" s="46" t="s">
+      <c r="B140" s="47" t="s">
         <v>227</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B141" s="46" t="s">
+      <c r="B141" s="47" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B142" s="46" t="s">
+      <c r="B142" s="47" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B143" s="46" t="s">
+      <c r="B143" s="47" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B144" s="46" t="s">
+      <c r="B144" s="47" t="s">
         <v>231</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B145" s="46" t="s">
+      <c r="B145" s="47" t="s">
         <v>232</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B146" s="46" t="s">
+      <c r="B146" s="47" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B147" s="46" t="s">
+      <c r="B147" s="47" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B148" s="46" t="s">
+      <c r="B148" s="47" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B149" s="46" t="s">
+      <c r="B149" s="47" t="s">
         <v>176</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B150" s="46" t="s">
+      <c r="B150" s="47" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B151" s="46" t="s">
+      <c r="B151" s="47" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B152" s="46" t="s">
+      <c r="B152" s="47" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B153" s="46" t="s">
+      <c r="B153" s="47" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B154" s="46" t="s">
+      <c r="B154" s="47" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B155" s="46" t="s">
+      <c r="B155" s="47" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B156" s="46" t="s">
+      <c r="B156" s="47" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B157" s="46" t="s">
+      <c r="B157" s="47" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B158" s="46" t="s">
+      <c r="B158" s="47" t="s">
         <v>233</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B159" s="46" t="s">
+      <c r="B159" s="47" t="s">
         <v>234</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B160" s="46" t="s">
+      <c r="B160" s="47" t="s">
         <v>235</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B161" s="46" t="s">
+      <c r="B161" s="47" t="s">
         <v>236</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B162" s="46" t="s">
+      <c r="B162" s="47" t="s">
         <v>237</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B163" s="46" t="s">
+      <c r="B163" s="47" t="s">
         <v>238</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B164" s="46" t="s">
+      <c r="B164" s="47" t="s">
         <v>239</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B165" s="46" t="s">
+      <c r="B165" s="47" t="s">
         <v>240</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B166" s="46" t="s">
+      <c r="B166" s="47" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B167" s="46" t="s">
+      <c r="B167" s="47" t="s">
         <v>242</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B168" s="46" t="s">
+      <c r="B168" s="47" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B169" s="46" t="s">
+      <c r="B169" s="47" t="s">
         <v>244</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B170" s="46" t="s">
+      <c r="B170" s="47" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B171" s="46" t="s">
+      <c r="B171" s="47" t="s">
         <v>187</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B172" s="46" t="s">
+      <c r="B172" s="47" t="s">
         <v>189</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B173" s="46" t="s">
+      <c r="B173" s="47" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B174" s="46" t="s">
+      <c r="B174" s="47" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B175" s="46" t="s">
+      <c r="B175" s="47" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B176" s="46" t="s">
+      <c r="B176" s="47" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B177" s="46" t="s">
+      <c r="B177" s="47" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B178" s="46" t="s">
+      <c r="B178" s="47" t="s">
         <v>201</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B179" s="46" t="s">
+      <c r="B179" s="47" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B180" s="46" t="s">
+      <c r="B180" s="47" t="s">
         <v>205</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B181" s="46" t="s">
+      <c r="B181" s="47" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B182" s="46" t="s">
+      <c r="B182" s="47" t="s">
         <v>245</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B183" s="46" t="s">
+      <c r="B183" s="47" t="s">
         <v>246</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B184" s="46" t="s">
+      <c r="B184" s="47" t="s">
         <v>247</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B185" s="46" t="s">
+      <c r="B185" s="47" t="s">
         <v>248</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B186" s="46" t="s">
+      <c r="B186" s="47" t="s">
         <v>249</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B187" s="46" t="s">
+      <c r="B187" s="47" t="s">
         <v>250</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B188" s="46" t="s">
+      <c r="B188" s="47" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B189" s="46" t="s">
+      <c r="B189" s="47" t="s">
         <v>252</v>
       </c>
     </row>
     <row r="190" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B190" s="46" t="s">
+      <c r="B190" s="47" t="s">
         <v>253</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B191" s="46" t="s">
+      <c r="B191" s="47" t="s">
         <v>254</v>
       </c>
     </row>
     <row r="192" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B192" s="46" t="s">
+      <c r="B192" s="47" t="s">
         <v>255</v>
       </c>
     </row>
     <row r="193" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B193" s="46" t="s">
+      <c r="B193" s="47" t="s">
         <v>256</v>
       </c>
     </row>
     <row r="194" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B194" s="46" t="s">
+      <c r="B194" s="47" t="s">
         <v>257</v>
       </c>
     </row>
     <row r="195" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B195" s="46" t="s">
+      <c r="B195" s="47" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="196" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B196" s="46" t="s">
+      <c r="B196" s="47" t="s">
         <v>259</v>
       </c>
     </row>
     <row r="197" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B197" s="46" t="s">
+      <c r="B197" s="47" t="s">
         <v>260</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B198" s="46" t="s">
+      <c r="B198" s="47" t="s">
         <v>261</v>
       </c>
     </row>
     <row r="199" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B199" s="46" t="s">
+      <c r="B199" s="47" t="s">
         <v>262</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B200" s="46" t="s">
+      <c r="B200" s="47" t="s">
         <v>263</v>
       </c>
     </row>
     <row r="201" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B201" s="46" t="s">
+      <c r="B201" s="47" t="s">
         <v>264</v>
       </c>
     </row>
     <row r="202" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B202" s="46" t="s">
+      <c r="B202" s="47" t="s">
         <v>265</v>
       </c>
     </row>
     <row r="203" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B203" s="46" t="s">
+      <c r="B203" s="47" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="204" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B204" s="46" t="s">
+      <c r="B204" s="47" t="s">
         <v>267</v>
       </c>
     </row>
     <row r="205" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B205" s="46" t="s">
+      <c r="B205" s="47" t="s">
         <v>268</v>
       </c>
     </row>
     <row r="206" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B206" s="46" t="s">
+      <c r="B206" s="47" t="s">
         <v>269</v>
       </c>
     </row>
     <row r="207" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B207" s="46" t="s">
+      <c r="B207" s="47" t="s">
         <v>270</v>
       </c>
     </row>
     <row r="208" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B208" s="46" t="s">
+      <c r="B208" s="47" t="s">
         <v>271</v>
       </c>
     </row>
     <row r="209" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B209" s="46" t="s">
+      <c r="B209" s="47" t="s">
         <v>272</v>
       </c>
     </row>
     <row r="210" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B210" s="46" t="s">
+      <c r="B210" s="47" t="s">
         <v>273</v>
       </c>
     </row>
     <row r="211" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B211" s="46" t="s">
+      <c r="B211" s="47" t="s">
         <v>274</v>
       </c>
     </row>
     <row r="212" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B212" s="46" t="s">
+      <c r="B212" s="47" t="s">
         <v>275</v>
       </c>
     </row>
     <row r="213" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B213" s="46" t="s">
+      <c r="B213" s="47" t="s">
         <v>276</v>
       </c>
     </row>
     <row r="214" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B214" s="46" t="s">
+      <c r="B214" s="47" t="s">
         <v>277</v>
       </c>
     </row>
     <row r="215" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B215" s="46" t="s">
+      <c r="B215" s="47" t="s">
         <v>278</v>
       </c>
     </row>
     <row r="216" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B216" s="46" t="s">
+      <c r="B216" s="47" t="s">
         <v>279</v>
       </c>
     </row>
     <row r="217" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B217" s="46" t="s">
+      <c r="B217" s="47" t="s">
         <v>280</v>
       </c>
     </row>
     <row r="218" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B218" s="46" t="s">
+      <c r="B218" s="47" t="s">
         <v>281</v>
       </c>
     </row>
     <row r="219" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B219" s="46" t="s">
+      <c r="B219" s="47" t="s">
         <v>282</v>
       </c>
     </row>
     <row r="220" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B220" s="46" t="s">
+      <c r="B220" s="47" t="s">
         <v>283</v>
       </c>
     </row>
     <row r="221" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B221" s="46" t="s">
+      <c r="B221" s="47" t="s">
         <v>284</v>
       </c>
     </row>
     <row r="222" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B222" s="46" t="s">
+      <c r="B222" s="47" t="s">
         <v>285</v>
       </c>
     </row>
     <row r="223" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B223" s="46" t="s">
+      <c r="B223" s="47" t="s">
         <v>286</v>
       </c>
     </row>
     <row r="224" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B224" s="46" t="s">
+      <c r="B224" s="47" t="s">
         <v>287</v>
       </c>
     </row>
     <row r="225" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B225" s="46" t="s">
+      <c r="B225" s="47" t="s">
         <v>288</v>
       </c>
     </row>
     <row r="226" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B226" s="46" t="s">
+      <c r="B226" s="47" t="s">
         <v>289</v>
       </c>
     </row>
     <row r="227" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B227" s="46" t="s">
+      <c r="B227" s="47" t="s">
         <v>290</v>
       </c>
     </row>
     <row r="228" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B228" s="46" t="s">
+      <c r="B228" s="47" t="s">
         <v>291</v>
       </c>
     </row>
     <row r="229" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B229" s="46" t="s">
+      <c r="B229" s="47" t="s">
         <v>292</v>
       </c>
     </row>
     <row r="230" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B230" s="46" t="s">
+      <c r="B230" s="47" t="s">
         <v>293</v>
       </c>
     </row>
     <row r="231" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B231" s="46" t="s">
+      <c r="B231" s="47" t="s">
         <v>294</v>
       </c>
     </row>
     <row r="232" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B232" s="46" t="s">
+      <c r="B232" s="47" t="s">
         <v>295</v>
       </c>
     </row>
     <row r="233" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B233" s="46" t="s">
+      <c r="B233" s="47" t="s">
         <v>296</v>
       </c>
     </row>
     <row r="234" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B234" s="46" t="s">
+      <c r="B234" s="47" t="s">
         <v>297</v>
       </c>
     </row>
     <row r="235" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B235" s="46" t="s">
+      <c r="B235" s="47" t="s">
         <v>298</v>
       </c>
     </row>
     <row r="236" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B236" s="46" t="s">
+      <c r="B236" s="47" t="s">
         <v>299</v>
       </c>
     </row>
     <row r="237" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B237" s="46" t="s">
+      <c r="B237" s="47" t="s">
         <v>300</v>
       </c>
     </row>
     <row r="238" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B238" s="46" t="s">
+      <c r="B238" s="47" t="s">
         <v>301</v>
       </c>
     </row>
     <row r="239" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B239" s="46" t="s">
+      <c r="B239" s="47" t="s">
         <v>302</v>
       </c>
     </row>
     <row r="240" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B240" s="46" t="s">
+      <c r="B240" s="47" t="s">
         <v>303</v>
       </c>
     </row>
     <row r="241" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B241" s="46" t="s">
+      <c r="B241" s="47" t="s">
         <v>304</v>
       </c>
     </row>
     <row r="242" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B242" s="46" t="s">
+      <c r="B242" s="47" t="s">
         <v>305</v>
       </c>
     </row>
     <row r="243" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B243" s="46" t="s">
+      <c r="B243" s="47" t="s">
         <v>306</v>
       </c>
     </row>
     <row r="244" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B244" s="46" t="s">
+      <c r="B244" s="47" t="s">
         <v>307</v>
       </c>
     </row>
     <row r="245" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B245" s="46" t="s">
+      <c r="B245" s="47" t="s">
         <v>308</v>
       </c>
     </row>
     <row r="246" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B246" s="46" t="s">
+      <c r="B246" s="47" t="s">
         <v>309</v>
       </c>
     </row>
     <row r="247" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B247" s="46" t="s">
+      <c r="B247" s="47" t="s">
         <v>310</v>
       </c>
     </row>
     <row r="248" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B248" s="46" t="s">
+      <c r="B248" s="47" t="s">
         <v>311</v>
       </c>
     </row>
     <row r="249" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B249" s="46" t="s">
+      <c r="B249" s="47" t="s">
         <v>312</v>
       </c>
     </row>
     <row r="250" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B250" s="46" t="s">
+      <c r="B250" s="47" t="s">
         <v>313</v>
       </c>
     </row>
     <row r="251" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B251" s="46" t="s">
+      <c r="B251" s="47" t="s">
         <v>314</v>
       </c>
     </row>
     <row r="252" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B252" s="46" t="s">
+      <c r="B252" s="47" t="s">
         <v>315</v>
       </c>
     </row>
     <row r="253" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B253" s="46" t="s">
+      <c r="B253" s="47" t="s">
         <v>316</v>
       </c>
     </row>
     <row r="254" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B254" s="46" t="s">
+      <c r="B254" s="47" t="s">
         <v>317</v>
       </c>
     </row>
     <row r="255" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B255" s="46" t="s">
+      <c r="B255" s="47" t="s">
         <v>318</v>
       </c>
     </row>
     <row r="256" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B256" s="46" t="s">
+      <c r="B256" s="47" t="s">
         <v>319</v>
       </c>
     </row>
     <row r="257" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B257" s="46" t="s">
+      <c r="B257" s="47" t="s">
         <v>320</v>
       </c>
     </row>
     <row r="258" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B258" s="46" t="s">
+      <c r="B258" s="47" t="s">
         <v>321</v>
       </c>
     </row>
     <row r="259" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B259" s="46" t="s">
+      <c r="B259" s="47" t="s">
         <v>322</v>
       </c>
     </row>
     <row r="260" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B260" s="46" t="s">
+      <c r="B260" s="47" t="s">
         <v>323</v>
       </c>
     </row>
     <row r="261" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B261" s="46" t="s">
+      <c r="B261" s="47" t="s">
         <v>324</v>
       </c>
     </row>
     <row r="262" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B262" s="46" t="s">
+      <c r="B262" s="47" t="s">
         <v>325</v>
       </c>
     </row>
     <row r="263" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B263" s="46" t="s">
+      <c r="B263" s="47" t="s">
         <v>326</v>
       </c>
     </row>
     <row r="264" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B264" s="46" t="s">
+      <c r="B264" s="47" t="s">
         <v>327</v>
       </c>
     </row>
     <row r="265" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B265" s="46" t="s">
+      <c r="B265" s="47" t="s">
         <v>328</v>
       </c>
     </row>
     <row r="266" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B266" s="46" t="s">
+      <c r="B266" s="47" t="s">
         <v>329</v>
       </c>
     </row>
     <row r="267" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B267" s="46" t="s">
+      <c r="B267" s="47" t="s">
         <v>330</v>
       </c>
     </row>
     <row r="268" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B268" s="46" t="s">
+      <c r="B268" s="47" t="s">
         <v>331</v>
       </c>
     </row>
     <row r="269" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B269" s="46" t="s">
+      <c r="B269" s="47" t="s">
         <v>332</v>
       </c>
     </row>
     <row r="270" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B270" s="46" t="s">
+      <c r="B270" s="47" t="s">
         <v>333</v>
       </c>
     </row>
     <row r="271" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B271" s="46" t="s">
+      <c r="B271" s="47" t="s">
         <v>334</v>
       </c>
     </row>
     <row r="272" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B272" s="46" t="s">
+      <c r="B272" s="47" t="s">
         <v>335</v>
       </c>
     </row>
     <row r="273" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B273" s="46" t="s">
+      <c r="B273" s="47" t="s">
         <v>336</v>
       </c>
     </row>
     <row r="274" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B274" s="46" t="s">
+      <c r="B274" s="47" t="s">
         <v>337</v>
       </c>
     </row>
     <row r="275" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B275" s="46" t="s">
+      <c r="B275" s="47" t="s">
         <v>338</v>
       </c>
     </row>
     <row r="276" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B276" s="46" t="s">
+      <c r="B276" s="47" t="s">
         <v>339</v>
       </c>
     </row>
     <row r="277" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B277" s="46" t="s">
+      <c r="B277" s="47" t="s">
         <v>340</v>
       </c>
     </row>
     <row r="278" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B278" s="46" t="s">
+      <c r="B278" s="47" t="s">
         <v>341</v>
       </c>
     </row>
     <row r="279" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B279" s="46" t="s">
+      <c r="B279" s="47" t="s">
         <v>342</v>
       </c>
     </row>
     <row r="280" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B280" s="46" t="s">
+      <c r="B280" s="47" t="s">
         <v>343</v>
       </c>
     </row>
     <row r="281" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B281" s="46" t="s">
+      <c r="B281" s="47" t="s">
         <v>344</v>
       </c>
     </row>
     <row r="282" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B282" s="46" t="s">
+      <c r="B282" s="47" t="s">
         <v>345</v>
       </c>
     </row>
     <row r="283" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B283" s="46" t="s">
+      <c r="B283" s="47" t="s">
         <v>346</v>
       </c>
     </row>
     <row r="284" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B284" s="46" t="s">
+      <c r="B284" s="47" t="s">
         <v>347</v>
       </c>
     </row>
     <row r="285" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B285" s="46" t="s">
+      <c r="B285" s="47" t="s">
         <v>348</v>
       </c>
     </row>
     <row r="286" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B286" s="46" t="s">
+      <c r="B286" s="47" t="s">
         <v>349</v>
       </c>
     </row>
     <row r="287" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B287" s="46" t="s">
+      <c r="B287" s="47" t="s">
         <v>350</v>
       </c>
     </row>
     <row r="288" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B288" s="46" t="s">
+      <c r="B288" s="47" t="s">
         <v>351</v>
       </c>
     </row>
     <row r="289" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B289" s="46" t="s">
+      <c r="B289" s="47" t="s">
         <v>352</v>
       </c>
     </row>
     <row r="290" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B290" s="46" t="s">
+      <c r="B290" s="47" t="s">
         <v>353</v>
       </c>
     </row>
     <row r="291" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B291" s="46" t="s">
+      <c r="B291" s="47" t="s">
         <v>354</v>
       </c>
     </row>
     <row r="292" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B292" s="46" t="s">
+      <c r="B292" s="47" t="s">
         <v>355</v>
       </c>
     </row>
     <row r="293" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B293" s="46" t="s">
+      <c r="B293" s="47" t="s">
         <v>356</v>
       </c>
     </row>
     <row r="294" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B294" s="46" t="s">
+      <c r="B294" s="47" t="s">
         <v>357</v>
       </c>
     </row>
     <row r="295" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B295" s="46" t="s">
+      <c r="B295" s="47" t="s">
         <v>358</v>
       </c>
     </row>
     <row r="296" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B296" s="46" t="s">
+      <c r="B296" s="47" t="s">
         <v>359</v>
       </c>
     </row>
     <row r="297" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B297" s="46" t="s">
+      <c r="B297" s="47" t="s">
         <v>360</v>
       </c>
     </row>
     <row r="298" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B298" s="46" t="s">
+      <c r="B298" s="47" t="s">
         <v>361</v>
       </c>
     </row>
     <row r="299" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B299" s="46" t="s">
+      <c r="B299" s="47" t="s">
         <v>362</v>
       </c>
     </row>
     <row r="300" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B300" s="46" t="s">
+      <c r="B300" s="47" t="s">
         <v>363</v>
       </c>
     </row>
     <row r="301" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B301" s="46" t="s">
+      <c r="B301" s="47" t="s">
         <v>364</v>
       </c>
     </row>
     <row r="302" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B302" s="46" t="s">
+      <c r="B302" s="47" t="s">
         <v>365</v>
       </c>
     </row>
     <row r="303" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B303" s="46" t="s">
+      <c r="B303" s="47" t="s">
         <v>366</v>
       </c>
     </row>
     <row r="304" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B304" s="46" t="s">
+      <c r="B304" s="47" t="s">
         <v>367</v>
       </c>
     </row>
     <row r="305" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B305" s="46" t="s">
+      <c r="B305" s="47" t="s">
         <v>368</v>
       </c>
     </row>
     <row r="306" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B306" s="46" t="s">
+      <c r="B306" s="47" t="s">
         <v>369</v>
       </c>
     </row>
     <row r="307" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B307" s="46" t="s">
+      <c r="B307" s="47" t="s">
         <v>370</v>
       </c>
     </row>
     <row r="308" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B308" s="46" t="s">
+      <c r="B308" s="47" t="s">
         <v>371</v>
       </c>
     </row>
     <row r="309" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B309" s="46" t="s">
+      <c r="B309" s="47" t="s">
         <v>372</v>
       </c>
     </row>
     <row r="310" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B310" s="46" t="s">
+      <c r="B310" s="47" t="s">
         <v>373</v>
       </c>
     </row>
     <row r="311" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B311" s="46" t="s">
+      <c r="B311" s="47" t="s">
         <v>374</v>
       </c>
     </row>
     <row r="312" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B312" s="46" t="s">
+      <c r="B312" s="47" t="s">
         <v>375</v>
       </c>
     </row>
     <row r="313" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B313" s="46" t="s">
+      <c r="B313" s="47" t="s">
         <v>376</v>
       </c>
     </row>
     <row r="314" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B314" s="46" t="s">
+      <c r="B314" s="47" t="s">
         <v>377</v>
       </c>
     </row>
     <row r="315" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B315" s="46" t="s">
+      <c r="B315" s="47" t="s">
         <v>378</v>
       </c>
     </row>
     <row r="316" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B316" s="46" t="s">
+      <c r="B316" s="47" t="s">
         <v>379</v>
       </c>
     </row>
     <row r="317" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B317" s="46" t="s">
+      <c r="B317" s="47" t="s">
         <v>380</v>
       </c>
     </row>
     <row r="318" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B318" s="46" t="s">
+      <c r="B318" s="47" t="s">
         <v>381</v>
       </c>
     </row>
     <row r="319" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B319" s="46" t="s">
+      <c r="B319" s="47" t="s">
         <v>382</v>
       </c>
     </row>
     <row r="320" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B320" s="46" t="s">
+      <c r="B320" s="47" t="s">
         <v>383</v>
       </c>
     </row>
     <row r="321" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B321" s="46" t="s">
+      <c r="B321" s="47" t="s">
         <v>384</v>
       </c>
     </row>
     <row r="322" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B322" s="46" t="s">
+      <c r="B322" s="47" t="s">
         <v>385</v>
       </c>
     </row>
     <row r="323" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B323" s="46" t="s">
+      <c r="B323" s="47" t="s">
         <v>386</v>
       </c>
     </row>
     <row r="324" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B324" s="46" t="s">
+      <c r="B324" s="47" t="s">
         <v>387</v>
       </c>
     </row>
     <row r="325" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B325" s="46" t="s">
+      <c r="B325" s="47" t="s">
         <v>388</v>
       </c>
     </row>
     <row r="326" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B326" s="46" t="s">
+      <c r="B326" s="47" t="s">
         <v>389</v>
       </c>
     </row>
     <row r="327" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B327" s="46" t="s">
+      <c r="B327" s="47" t="s">
         <v>390</v>
       </c>
     </row>
     <row r="328" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B328" s="46" t="s">
+      <c r="B328" s="47" t="s">
         <v>391</v>
       </c>
     </row>
     <row r="329" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B329" s="46" t="s">
+      <c r="B329" s="47" t="s">
         <v>392</v>
       </c>
     </row>
     <row r="330" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B330" s="46" t="s">
+      <c r="B330" s="47" t="s">
         <v>393</v>
       </c>
     </row>
     <row r="331" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B331" s="46" t="s">
+      <c r="B331" s="47" t="s">
         <v>394</v>
       </c>
     </row>
     <row r="332" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B332" s="46" t="s">
+      <c r="B332" s="47" t="s">
         <v>395</v>
       </c>
     </row>
     <row r="333" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B333" s="46" t="s">
+      <c r="B333" s="47" t="s">
         <v>396</v>
       </c>
     </row>
     <row r="334" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B334" s="46" t="s">
+      <c r="B334" s="47" t="s">
         <v>397</v>
       </c>
     </row>
     <row r="335" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B335" s="46" t="s">
+      <c r="B335" s="47" t="s">
         <v>398</v>
       </c>
     </row>
     <row r="336" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B336" s="46" t="s">
+      <c r="B336" s="47" t="s">
         <v>399</v>
       </c>
     </row>
     <row r="337" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B337" s="46" t="s">
+      <c r="B337" s="47" t="s">
         <v>400</v>
       </c>
     </row>
     <row r="338" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B338" s="46" t="s">
+      <c r="B338" s="47" t="s">
         <v>401</v>
       </c>
     </row>
     <row r="339" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B339" s="46" t="s">
+      <c r="B339" s="47" t="s">
         <v>402</v>
       </c>
     </row>
     <row r="340" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B340" s="46" t="s">
+      <c r="B340" s="47" t="s">
         <v>403</v>
       </c>
     </row>
     <row r="341" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B341" s="46" t="s">
+      <c r="B341" s="47" t="s">
         <v>404</v>
       </c>
     </row>
     <row r="342" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B342" s="46" t="s">
+      <c r="B342" s="47" t="s">
         <v>405</v>
       </c>
     </row>
     <row r="343" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B343" s="46" t="s">
+      <c r="B343" s="47" t="s">
         <v>406</v>
       </c>
     </row>
     <row r="344" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B344" s="46" t="s">
+      <c r="B344" s="47" t="s">
         <v>407</v>
       </c>
     </row>
     <row r="345" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B345" s="46" t="s">
+      <c r="B345" s="47" t="s">
         <v>408</v>
       </c>
     </row>
     <row r="346" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B346" s="46" t="s">
+      <c r="B346" s="47" t="s">
         <v>409</v>
       </c>
     </row>
     <row r="347" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B347" s="46" t="s">
+      <c r="B347" s="47" t="s">
         <v>410</v>
       </c>
     </row>
     <row r="348" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B348" s="46" t="s">
+      <c r="B348" s="47" t="s">
         <v>411</v>
       </c>
     </row>
     <row r="349" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B349" s="46" t="s">
+      <c r="B349" s="47" t="s">
         <v>412</v>
       </c>
     </row>
     <row r="350" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B350" s="46" t="s">
+      <c r="B350" s="47" t="s">
         <v>413</v>
       </c>
     </row>
     <row r="351" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B351" s="46" t="s">
+      <c r="B351" s="47" t="s">
         <v>414</v>
       </c>
     </row>
     <row r="352" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B352" s="46" t="s">
+      <c r="B352" s="47" t="s">
         <v>415</v>
       </c>
     </row>
     <row r="353" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B353" s="46" t="s">
+      <c r="B353" s="47" t="s">
         <v>416</v>
       </c>
     </row>
     <row r="354" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B354" s="46" t="s">
+      <c r="B354" s="47" t="s">
         <v>417</v>
       </c>
     </row>
     <row r="355" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B355" s="46" t="s">
+      <c r="B355" s="47" t="s">
         <v>418</v>
       </c>
     </row>
     <row r="356" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B356" s="46" t="s">
+      <c r="B356" s="47" t="s">
         <v>419</v>
       </c>
     </row>
     <row r="357" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B357" s="46" t="s">
+      <c r="B357" s="47" t="s">
         <v>420</v>
       </c>
     </row>
     <row r="358" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B358" s="46" t="s">
+      <c r="B358" s="47" t="s">
         <v>421</v>
       </c>
     </row>
     <row r="359" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B359" s="46" t="s">
+      <c r="B359" s="47" t="s">
         <v>422</v>
       </c>
     </row>
     <row r="360" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B360" s="46" t="s">
+      <c r="B360" s="47" t="s">
         <v>423</v>
       </c>
     </row>
     <row r="361" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B361" s="46" t="s">
+      <c r="B361" s="47" t="s">
         <v>424</v>
       </c>
     </row>
     <row r="362" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B362" s="46" t="s">
+      <c r="B362" s="47" t="s">
         <v>425</v>
       </c>
     </row>
     <row r="363" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B363" s="46" t="s">
+      <c r="B363" s="47" t="s">
         <v>426</v>
       </c>
     </row>
     <row r="364" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B364" s="46" t="s">
+      <c r="B364" s="47" t="s">
         <v>427</v>
       </c>
     </row>
     <row r="365" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B365" s="46" t="s">
+      <c r="B365" s="47" t="s">
         <v>428</v>
       </c>
     </row>
     <row r="366" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B366" s="46" t="s">
+      <c r="B366" s="47" t="s">
         <v>429</v>
       </c>
     </row>
     <row r="367" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B367" s="46" t="s">
+      <c r="B367" s="47" t="s">
         <v>430</v>
       </c>
     </row>
     <row r="368" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B368" s="46" t="s">
+      <c r="B368" s="47" t="s">
         <v>431</v>
       </c>
     </row>
     <row r="369" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B369" s="46" t="s">
+      <c r="B369" s="47" t="s">
         <v>432</v>
       </c>
     </row>
     <row r="370" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B370" s="46" t="s">
+      <c r="B370" s="47" t="s">
         <v>433</v>
       </c>
     </row>
     <row r="371" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B371" s="46" t="s">
+      <c r="B371" s="47" t="s">
         <v>434</v>
       </c>
     </row>
     <row r="372" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B372" s="46" t="s">
+      <c r="B372" s="47" t="s">
         <v>435</v>
       </c>
     </row>
     <row r="373" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B373" s="46" t="s">
+      <c r="B373" s="47" t="s">
         <v>436</v>
       </c>
     </row>
     <row r="374" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B374" s="46" t="s">
+      <c r="B374" s="47" t="s">
         <v>437</v>
       </c>
     </row>
     <row r="375" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B375" s="46" t="s">
+      <c r="B375" s="47" t="s">
         <v>438</v>
       </c>
     </row>
     <row r="376" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B376" s="46" t="s">
+      <c r="B376" s="47" t="s">
         <v>439</v>
       </c>
     </row>
     <row r="377" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B377" s="46" t="s">
+      <c r="B377" s="47" t="s">
         <v>440</v>
       </c>
     </row>
     <row r="378" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B378" s="46" t="s">
+      <c r="B378" s="47" t="s">
         <v>441</v>
       </c>
     </row>
     <row r="379" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B379" s="46" t="s">
+      <c r="B379" s="47" t="s">
         <v>442</v>
       </c>
     </row>
     <row r="380" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B380" s="46" t="s">
+      <c r="B380" s="47" t="s">
         <v>443</v>
       </c>
     </row>
     <row r="381" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B381" s="46" t="s">
+      <c r="B381" s="47" t="s">
         <v>444</v>
       </c>
     </row>
     <row r="382" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B382" s="46" t="s">
+      <c r="B382" s="47" t="s">
         <v>445</v>
       </c>
     </row>
     <row r="383" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B383" s="46" t="s">
+      <c r="B383" s="47" t="s">
         <v>446</v>
       </c>
     </row>
     <row r="384" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B384" s="46" t="s">
+      <c r="B384" s="47" t="s">
         <v>447</v>
       </c>
     </row>
     <row r="385" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B385" s="46" t="s">
+      <c r="B385" s="47" t="s">
         <v>448</v>
       </c>
     </row>
@@ -29855,8 +29749,8 @@
     <row r="1000" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
Applied first row formula to all rows.
</commit_message>
<xml_diff>
--- a/backend/fms_core/static/submission_templates/Library_QC_v4_8_0.xlsx
+++ b/backend/fms_core/static/submission_templates/Library_QC_v4_8_0.xlsx
@@ -28,7 +28,7 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
-    <author>UFG</author>
+    <author> </author>
   </authors>
   <commentList>
     <comment ref="E5" authorId="0">
@@ -1815,7 +1815,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2004,7 +2004,7 @@
       <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.55078125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="25.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="27.88"/>
@@ -2217,7 +2217,7 @@
       <c r="I9" s="17"/>
       <c r="J9" s="17"/>
       <c r="K9" s="18" t="str">
-        <f aca="true">IF(AND(AND(ISBLANK(D9), ISBLANK(E9)),AND(OR(ISBLANK(G9),ISBLANK(H9),ISBLANK(I9)))),"",IF(ISBLANK(J9),IF(ISBLANK(E9),(D9-F9)*I9*H9*INDIRECT(SUBSTITUTE(G9," ","_"))/1000000,(E9-F9)*I9*H9*INDIRECT(SUBSTITUTE(G9," ","_"))/1000000),IF(ISBLANK(E9),(D9-F9)*J9,(E9-F9)*J9)))</f>
+        <f aca="true">IF(OR(AND(ISBLANK(D9), ISBLANK(E9)),AND(OR(ISBLANK(G9),ISBLANK(H9),ISBLANK(I9)),ISBLANK(J9))),"",IF(ISBLANK(J9),IF(ISBLANK(E9),(D9-F9)*I9*H9*INDIRECT(SUBSTITUTE(G9," ","_"))/1000000,(E9-F9)*I9*H9*INDIRECT(SUBSTITUTE(G9," ","_"))/1000000),IF(ISBLANK(E9),(D9-F9)*J9,(E9-F9)*J9)))</f>
         <v/>
       </c>
       <c r="L9" s="15"/>
@@ -2262,7 +2262,10 @@
       <c r="H11" s="17"/>
       <c r="I11" s="17"/>
       <c r="J11" s="17"/>
-      <c r="K11" s="22"/>
+      <c r="K11" s="22" t="str">
+        <f aca="true">IF(OR(AND(ISBLANK(D11), ISBLANK(E11)),AND(OR(ISBLANK(G11),ISBLANK(H11),ISBLANK(I11)),ISBLANK(J11))),"",IF(ISBLANK(J11),IF(ISBLANK(E11),(D11-F11)*I11*H11*INDIRECT(SUBSTITUTE(G11," ","_"))/1000000,(E11-F11)*I11*H11*INDIRECT(SUBSTITUTE(G11," ","_"))/1000000),IF(ISBLANK(E11),(D11-F11)*J11,(E11-F11)*J11)))</f>
+        <v/>
+      </c>
       <c r="L11" s="15"/>
       <c r="M11" s="15"/>
       <c r="N11" s="15"/>
@@ -25063,7 +25066,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.46875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.4609375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="47.19"/>
   </cols>
@@ -26782,7 +26785,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.55078125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="9.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="16.5"/>

</xml_diff>

<commit_message>
Added Femto Pulse as quality instrument.
</commit_message>
<xml_diff>
--- a/backend/fms_core/static/submission_templates/Library_QC_v4_8_0.xlsx
+++ b/backend/fms_core/static/submission_templates/Library_QC_v4_8_0.xlsx
@@ -28,7 +28,7 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
-    <author> </author>
+    <author>UFG</author>
   </authors>
   <commentList>
     <comment ref="E5" authorId="0">
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="575" uniqueCount="449">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="450">
   <si>
     <t xml:space="preserve">Library QC Template</t>
   </si>
@@ -276,6 +276,9 @@
   </si>
   <si>
     <t xml:space="preserve">A03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Femto Pulse</t>
   </si>
   <si>
     <t xml:space="preserve">Repeat QC step - Repeat current QC step</t>
@@ -2000,7 +2003,7 @@
       <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.52734375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="25.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="27.88"/>
@@ -25031,12 +25034,12 @@
       <formula1>Index!$K$2:$K$5</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="L6:L1000" type="list">
-      <formula1>Index!$D$2:$D$3</formula1>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="N6:N1000" type="list">
+      <formula1>Index!$E$2:$E$3</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="N6:N1000" type="list">
-      <formula1>Index!$E$2:$E$3</formula1>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="L6:L1000" type="list">
+      <formula1>Index!$D$2:$D$4</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -25062,7 +25065,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.4453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="47.19"/>
   </cols>
@@ -26781,7 +26784,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.52734375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="9.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="16.5"/>
@@ -26891,7 +26894,9 @@
         <v>65</v>
       </c>
       <c r="C4" s="46"/>
-      <c r="D4" s="46"/>
+      <c r="D4" s="46" t="s">
+        <v>66</v>
+      </c>
       <c r="E4" s="46"/>
       <c r="F4" s="46"/>
       <c r="G4" s="46"/>
@@ -26899,15 +26904,15 @@
       <c r="I4" s="46"/>
       <c r="J4" s="46"/>
       <c r="K4" s="46" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="46" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B5" s="46" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C5" s="46"/>
       <c r="E5" s="46"/>
@@ -26917,15 +26922,15 @@
       <c r="I5" s="46"/>
       <c r="J5" s="46"/>
       <c r="K5" s="46" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="46" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B6" s="46" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C6" s="46"/>
       <c r="D6" s="46"/>
@@ -26939,10 +26944,10 @@
     </row>
     <row r="7" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="46" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B7" s="46" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C7" s="46"/>
       <c r="D7" s="46"/>
@@ -26956,10 +26961,10 @@
     </row>
     <row r="8" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="46" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B8" s="46" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C8" s="46"/>
       <c r="D8" s="46"/>
@@ -26973,10 +26978,10 @@
     </row>
     <row r="9" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="46" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B9" s="46" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C9" s="46"/>
       <c r="E9" s="46"/>
@@ -26984,2151 +26989,2151 @@
     </row>
     <row r="10" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="46" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B10" s="46" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C10" s="46"/>
     </row>
     <row r="11" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="46" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B11" s="46" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C11" s="46"/>
     </row>
     <row r="12" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="46" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B12" s="46" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C12" s="46"/>
     </row>
     <row r="13" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="46" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B13" s="46" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C13" s="46"/>
     </row>
     <row r="14" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="46" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B14" s="46" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C14" s="46"/>
     </row>
     <row r="15" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="46" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B15" s="46" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="46" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B16" s="46" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="46" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B17" s="46" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="46" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B18" s="46" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="46" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B19" s="46" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="46" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B20" s="46" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="46" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B21" s="46" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="46" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B22" s="46" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="46" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B23" s="46" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="46" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B24" s="46" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="46" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B25" s="46" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="46" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B26" s="46" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="46" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B27" s="46" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="46" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B28" s="46" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="46" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B29" s="46" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="46" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B30" s="46" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="46" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B31" s="46" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="46" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B32" s="46" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="46" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B33" s="46" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="46" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B34" s="46" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="46" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B35" s="46" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="46" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B36" s="46" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="46" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B37" s="46" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="46" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B38" s="46" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="46" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B39" s="46" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="46" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B40" s="46" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="46" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B41" s="46" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="46" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B42" s="46" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="46" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B43" s="46" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="46" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B44" s="46" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="46" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B45" s="46" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="46" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B46" s="46" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="46" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B47" s="46" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="46" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B48" s="46" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="46" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B49" s="46" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="46" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B50" s="46" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="46" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B51" s="46" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="46" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B52" s="46" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="46" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B53" s="46" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="46" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B54" s="46" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="46" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B55" s="46" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="46" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B56" s="46" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="46" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B57" s="46" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="46" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B58" s="46" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="46" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B59" s="46" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="46" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B60" s="46" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="46" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B61" s="46" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="46" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B62" s="46" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="46" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B63" s="46" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="46" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B64" s="46" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="46" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B65" s="46" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="46" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B66" s="46" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="46" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B67" s="46" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A68" s="46" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B68" s="46" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="46" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B69" s="46" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="46" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B70" s="46" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="46" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B71" s="46" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="46" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B72" s="46" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="46" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B73" s="46" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="46" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B74" s="46" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="46" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B75" s="46" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="46" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B76" s="46" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A77" s="46" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B77" s="46" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A78" s="46" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B78" s="46" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A79" s="46" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B79" s="46" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A80" s="46" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B80" s="46" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A81" s="46" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B81" s="46" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A82" s="46" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B82" s="46" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A83" s="46" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B83" s="46" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A84" s="46" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B84" s="46" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A85" s="46" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B85" s="46" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A86" s="46" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B86" s="46" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A87" s="46" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B87" s="46" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A88" s="46" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B88" s="46" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A89" s="46" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B89" s="46" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A90" s="46" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B90" s="46" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A91" s="46" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B91" s="46" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A92" s="46" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B92" s="46" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A93" s="46" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B93" s="46" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A94" s="46" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B94" s="46" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A95" s="46" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B95" s="46" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A96" s="46" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B96" s="46" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A97" s="46" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B97" s="46" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B98" s="46" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B99" s="46" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B100" s="46" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B101" s="46" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B102" s="46" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B103" s="46" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B104" s="46" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B105" s="46" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B106" s="46" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B107" s="46" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B108" s="46" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B109" s="46" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B110" s="46" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B111" s="46" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B112" s="46" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B113" s="46" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B114" s="46" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B115" s="46" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B116" s="46" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B117" s="46" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B118" s="46" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B119" s="46" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B120" s="46" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B121" s="46" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B122" s="46" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B123" s="46" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B124" s="46" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B125" s="46" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B126" s="46" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B127" s="46" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B128" s="46" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B129" s="46" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B130" s="46" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B131" s="46" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B132" s="46" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B133" s="46" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B134" s="46" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B135" s="46" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B136" s="46" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B137" s="46" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B138" s="46" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B139" s="46" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B140" s="46" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B141" s="46" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B142" s="46" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B143" s="46" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B144" s="46" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B145" s="46" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B146" s="46" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B147" s="46" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B148" s="46" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B149" s="46" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B150" s="46" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B151" s="46" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B152" s="46" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B153" s="46" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B154" s="46" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B155" s="46" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B156" s="46" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B157" s="46" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B158" s="46" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B159" s="46" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B160" s="46" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B161" s="46" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B162" s="46" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B163" s="46" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B164" s="46" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B165" s="46" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B166" s="46" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B167" s="46" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B168" s="46" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B169" s="46" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B170" s="46" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B171" s="46" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B172" s="46" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B173" s="46" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B174" s="46" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B175" s="46" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B176" s="46" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B177" s="46" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B178" s="46" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B179" s="46" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B180" s="46" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B181" s="46" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B182" s="46" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B183" s="46" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B184" s="46" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B185" s="46" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B186" s="46" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B187" s="46" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B188" s="46" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B189" s="46" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
     </row>
     <row r="190" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B190" s="46" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B191" s="46" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
     </row>
     <row r="192" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B192" s="46" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
     </row>
     <row r="193" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B193" s="46" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
     </row>
     <row r="194" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B194" s="46" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
     </row>
     <row r="195" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B195" s="46" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row r="196" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B196" s="46" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="197" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B197" s="46" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B198" s="46" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="199" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B199" s="46" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B200" s="46" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="201" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B201" s="46" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="202" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B202" s="46" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="203" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B203" s="46" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
     <row r="204" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B204" s="46" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="205" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B205" s="46" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="206" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B206" s="46" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
     <row r="207" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B207" s="46" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="208" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B208" s="46" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row r="209" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B209" s="46" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="210" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B210" s="46" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="211" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B211" s="46" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="212" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B212" s="46" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="213" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B213" s="46" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="214" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B214" s="46" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="215" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B215" s="46" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="216" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B216" s="46" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="217" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B217" s="46" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
     </row>
     <row r="218" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B218" s="46" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row r="219" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B219" s="46" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
     </row>
     <row r="220" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B220" s="46" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
     </row>
     <row r="221" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B221" s="46" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
     </row>
     <row r="222" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B222" s="46" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
     </row>
     <row r="223" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B223" s="46" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
     </row>
     <row r="224" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B224" s="46" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
     </row>
     <row r="225" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B225" s="46" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
     </row>
     <row r="226" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B226" s="46" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
     </row>
     <row r="227" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B227" s="46" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
     </row>
     <row r="228" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B228" s="46" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="229" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B229" s="46" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
     </row>
     <row r="230" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B230" s="46" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
     </row>
     <row r="231" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B231" s="46" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
     </row>
     <row r="232" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B232" s="46" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="233" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B233" s="46" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
     </row>
     <row r="234" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B234" s="46" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
     </row>
     <row r="235" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B235" s="46" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
     </row>
     <row r="236" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B236" s="46" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
     </row>
     <row r="237" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B237" s="46" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
     </row>
     <row r="238" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B238" s="46" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
     </row>
     <row r="239" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B239" s="46" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
     </row>
     <row r="240" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B240" s="46" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
     </row>
     <row r="241" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B241" s="46" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
     </row>
     <row r="242" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B242" s="46" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
     </row>
     <row r="243" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B243" s="46" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
     </row>
     <row r="244" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B244" s="46" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
     </row>
     <row r="245" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B245" s="46" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
     </row>
     <row r="246" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B246" s="46" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
     </row>
     <row r="247" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B247" s="46" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
     </row>
     <row r="248" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B248" s="46" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
     </row>
     <row r="249" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B249" s="46" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
     </row>
     <row r="250" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B250" s="46" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
     </row>
     <row r="251" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B251" s="46" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
     </row>
     <row r="252" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B252" s="46" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
     </row>
     <row r="253" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B253" s="46" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row r="254" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B254" s="46" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
     </row>
     <row r="255" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B255" s="46" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
     </row>
     <row r="256" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B256" s="46" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
     </row>
     <row r="257" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B257" s="46" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
     </row>
     <row r="258" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B258" s="46" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
     </row>
     <row r="259" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B259" s="46" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
     </row>
     <row r="260" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B260" s="46" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
     </row>
     <row r="261" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B261" s="46" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
     </row>
     <row r="262" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B262" s="46" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
     </row>
     <row r="263" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B263" s="46" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
     </row>
     <row r="264" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B264" s="46" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
     </row>
     <row r="265" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B265" s="46" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
     </row>
     <row r="266" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B266" s="46" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
     </row>
     <row r="267" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B267" s="46" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
     </row>
     <row r="268" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B268" s="46" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
     </row>
     <row r="269" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B269" s="46" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
     </row>
     <row r="270" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B270" s="46" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
     </row>
     <row r="271" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B271" s="46" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
     </row>
     <row r="272" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B272" s="46" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
     </row>
     <row r="273" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B273" s="46" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
     </row>
     <row r="274" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B274" s="46" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
     </row>
     <row r="275" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B275" s="46" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
     </row>
     <row r="276" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B276" s="46" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
     </row>
     <row r="277" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B277" s="46" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
     </row>
     <row r="278" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B278" s="46" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
     </row>
     <row r="279" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B279" s="46" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
     </row>
     <row r="280" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B280" s="46" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="281" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B281" s="46" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
     </row>
     <row r="282" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B282" s="46" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
     </row>
     <row r="283" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B283" s="46" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
     </row>
     <row r="284" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B284" s="46" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="285" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B285" s="46" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
     </row>
     <row r="286" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B286" s="46" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
     </row>
     <row r="287" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B287" s="46" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
     </row>
     <row r="288" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B288" s="46" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
     </row>
     <row r="289" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B289" s="46" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
     </row>
     <row r="290" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B290" s="46" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
     </row>
     <row r="291" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B291" s="46" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
     </row>
     <row r="292" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B292" s="46" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
     </row>
     <row r="293" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B293" s="46" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
     </row>
     <row r="294" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B294" s="46" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
     </row>
     <row r="295" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B295" s="46" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
     </row>
     <row r="296" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B296" s="46" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
     </row>
     <row r="297" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B297" s="46" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
     </row>
     <row r="298" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B298" s="46" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
     </row>
     <row r="299" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B299" s="46" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
     </row>
     <row r="300" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B300" s="46" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
     </row>
     <row r="301" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B301" s="46" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
     </row>
     <row r="302" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B302" s="46" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
     </row>
     <row r="303" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B303" s="46" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
     </row>
     <row r="304" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B304" s="46" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
     </row>
     <row r="305" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B305" s="46" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
     </row>
     <row r="306" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B306" s="46" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
     </row>
     <row r="307" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B307" s="46" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
     </row>
     <row r="308" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B308" s="46" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
     </row>
     <row r="309" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B309" s="46" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
     </row>
     <row r="310" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B310" s="46" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
     </row>
     <row r="311" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B311" s="46" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
     </row>
     <row r="312" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B312" s="46" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
     </row>
     <row r="313" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B313" s="46" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
     </row>
     <row r="314" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B314" s="46" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
     </row>
     <row r="315" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B315" s="46" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
     </row>
     <row r="316" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B316" s="46" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
     </row>
     <row r="317" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B317" s="46" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
     </row>
     <row r="318" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B318" s="46" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
     </row>
     <row r="319" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B319" s="46" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
     </row>
     <row r="320" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B320" s="46" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="321" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B321" s="46" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
     </row>
     <row r="322" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B322" s="46" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
     </row>
     <row r="323" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B323" s="46" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
     </row>
     <row r="324" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B324" s="46" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
     </row>
     <row r="325" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B325" s="46" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
     </row>
     <row r="326" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B326" s="46" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
     </row>
     <row r="327" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B327" s="46" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
     </row>
     <row r="328" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B328" s="46" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
     </row>
     <row r="329" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B329" s="46" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
     </row>
     <row r="330" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B330" s="46" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
     </row>
     <row r="331" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B331" s="46" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
     </row>
     <row r="332" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B332" s="46" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="333" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B333" s="46" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
     </row>
     <row r="334" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B334" s="46" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
     </row>
     <row r="335" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B335" s="46" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
     </row>
     <row r="336" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B336" s="46" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
     </row>
     <row r="337" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B337" s="46" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
     </row>
     <row r="338" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B338" s="46" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
     </row>
     <row r="339" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B339" s="46" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
     </row>
     <row r="340" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B340" s="46" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
     </row>
     <row r="341" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B341" s="46" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
     </row>
     <row r="342" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B342" s="46" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
     </row>
     <row r="343" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B343" s="46" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
     </row>
     <row r="344" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B344" s="46" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
     </row>
     <row r="345" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B345" s="46" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
     </row>
     <row r="346" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B346" s="46" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
     </row>
     <row r="347" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B347" s="46" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
     </row>
     <row r="348" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B348" s="46" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
     </row>
     <row r="349" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B349" s="46" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
     </row>
     <row r="350" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B350" s="46" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
     </row>
     <row r="351" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B351" s="46" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
     </row>
     <row r="352" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B352" s="46" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
     </row>
     <row r="353" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B353" s="46" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
     </row>
     <row r="354" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B354" s="46" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
     </row>
     <row r="355" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B355" s="46" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
     </row>
     <row r="356" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B356" s="46" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="357" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B357" s="46" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
     </row>
     <row r="358" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B358" s="46" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
     </row>
     <row r="359" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B359" s="46" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
     </row>
     <row r="360" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B360" s="46" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
     </row>
     <row r="361" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B361" s="46" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
     </row>
     <row r="362" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B362" s="46" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
     </row>
     <row r="363" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B363" s="46" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
     </row>
     <row r="364" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B364" s="46" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
     </row>
     <row r="365" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B365" s="46" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
     </row>
     <row r="366" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B366" s="46" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
     </row>
     <row r="367" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B367" s="46" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
     </row>
     <row r="368" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B368" s="46" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
     </row>
     <row r="369" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B369" s="46" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
     </row>
     <row r="370" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B370" s="46" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
     </row>
     <row r="371" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B371" s="46" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
     </row>
     <row r="372" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B372" s="46" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
     </row>
     <row r="373" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B373" s="46" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
     </row>
     <row r="374" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B374" s="46" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
     </row>
     <row r="375" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B375" s="46" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
     </row>
     <row r="376" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B376" s="46" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
     </row>
     <row r="377" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B377" s="46" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
     </row>
     <row r="378" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B378" s="46" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
     </row>
     <row r="379" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B379" s="46" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
     </row>
     <row r="380" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B380" s="46" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
     </row>
     <row r="381" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B381" s="46" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
     </row>
     <row r="382" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B382" s="46" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
     </row>
     <row r="383" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B383" s="46" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
     </row>
     <row r="384" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B384" s="46" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
     </row>
     <row r="385" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B385" s="46" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
     </row>
     <row r="386" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Add a list of non instrument exception for quality instruments. Modified the lib qc template. Update the prefiling values.
</commit_message>
<xml_diff>
--- a/backend/fms_core/static/submission_templates/Library_QC_v4_8_0.xlsx
+++ b/backend/fms_core/static/submission_templates/Library_QC_v4_8_0.xlsx
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="450">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="577" uniqueCount="451">
   <si>
     <t xml:space="preserve">Library QC Template</t>
   </si>
@@ -285,6 +285,9 @@
   </si>
   <si>
     <t xml:space="preserve">A04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N/A - WGS Tagmentation</t>
   </si>
   <si>
     <t xml:space="preserve">Ignore workflow - Do not register as part of a workflow</t>
@@ -2003,7 +2006,7 @@
       <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.52734375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.51953125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="25.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="27.88"/>
@@ -25039,7 +25042,7 @@
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="L6:L1000" type="list">
-      <formula1>Index!$D$2:$D$4</formula1>
+      <formula1>Index!$D$2:$D$5</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -25065,7 +25068,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.4453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.4375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="47.19"/>
   </cols>
@@ -26784,11 +26787,11 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.52734375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.51953125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="9.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="16.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="22.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="31.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="26.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="17.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="9.4"/>
@@ -26915,6 +26918,9 @@
         <v>68</v>
       </c>
       <c r="C5" s="46"/>
+      <c r="D5" s="1" t="s">
+        <v>69</v>
+      </c>
       <c r="E5" s="46"/>
       <c r="F5" s="46"/>
       <c r="G5" s="46"/>
@@ -26922,15 +26928,15 @@
       <c r="I5" s="46"/>
       <c r="J5" s="46"/>
       <c r="K5" s="46" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="46" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B6" s="46" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C6" s="46"/>
       <c r="D6" s="46"/>
@@ -26944,10 +26950,10 @@
     </row>
     <row r="7" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="46" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B7" s="46" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C7" s="46"/>
       <c r="D7" s="46"/>
@@ -26961,10 +26967,10 @@
     </row>
     <row r="8" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="46" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B8" s="46" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C8" s="46"/>
       <c r="D8" s="46"/>
@@ -26978,10 +26984,10 @@
     </row>
     <row r="9" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="46" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B9" s="46" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C9" s="46"/>
       <c r="E9" s="46"/>
@@ -26989,2151 +26995,2151 @@
     </row>
     <row r="10" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="46" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B10" s="46" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C10" s="46"/>
     </row>
     <row r="11" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="46" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B11" s="46" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C11" s="46"/>
     </row>
     <row r="12" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="46" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B12" s="46" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C12" s="46"/>
     </row>
     <row r="13" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="46" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B13" s="46" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C13" s="46"/>
     </row>
     <row r="14" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="46" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B14" s="46" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C14" s="46"/>
     </row>
     <row r="15" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="46" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B15" s="46" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="46" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B16" s="46" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="46" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B17" s="46" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="46" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B18" s="46" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="46" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B19" s="46" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="46" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B20" s="46" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="46" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B21" s="46" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="46" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B22" s="46" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="46" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B23" s="46" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="46" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B24" s="46" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="46" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B25" s="46" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="46" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B26" s="46" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="46" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B27" s="46" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="46" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B28" s="46" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="46" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B29" s="46" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="46" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B30" s="46" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="46" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B31" s="46" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="46" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B32" s="46" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="46" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B33" s="46" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="46" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B34" s="46" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="46" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B35" s="46" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="46" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B36" s="46" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="46" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B37" s="46" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="46" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B38" s="46" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="46" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B39" s="46" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="46" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B40" s="46" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="46" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B41" s="46" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="46" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B42" s="46" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="46" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B43" s="46" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="46" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B44" s="46" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="46" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B45" s="46" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="46" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B46" s="46" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="46" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B47" s="46" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="46" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B48" s="46" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="46" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B49" s="46" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="46" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B50" s="46" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="46" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B51" s="46" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="46" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B52" s="46" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="46" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B53" s="46" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="46" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B54" s="46" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="46" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B55" s="46" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="46" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B56" s="46" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="46" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B57" s="46" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="46" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B58" s="46" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="46" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B59" s="46" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="46" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B60" s="46" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="46" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B61" s="46" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="46" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B62" s="46" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="46" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B63" s="46" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="46" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B64" s="46" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="46" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B65" s="46" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="46" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B66" s="46" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="46" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B67" s="46" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A68" s="46" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B68" s="46" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="46" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B69" s="46" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="46" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B70" s="46" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="46" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B71" s="46" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="46" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B72" s="46" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="46" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B73" s="46" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="46" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B74" s="46" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="46" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B75" s="46" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="46" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B76" s="46" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A77" s="46" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B77" s="46" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A78" s="46" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B78" s="46" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A79" s="46" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B79" s="46" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A80" s="46" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B80" s="46" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A81" s="46" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B81" s="46" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A82" s="46" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B82" s="46" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A83" s="46" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B83" s="46" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A84" s="46" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B84" s="46" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A85" s="46" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B85" s="46" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A86" s="46" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B86" s="46" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A87" s="46" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B87" s="46" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A88" s="46" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B88" s="46" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A89" s="46" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B89" s="46" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A90" s="46" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B90" s="46" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A91" s="46" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B91" s="46" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A92" s="46" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B92" s="46" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A93" s="46" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B93" s="46" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A94" s="46" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B94" s="46" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A95" s="46" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B95" s="46" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A96" s="46" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B96" s="46" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A97" s="46" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B97" s="46" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B98" s="46" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B99" s="46" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B100" s="46" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B101" s="46" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B102" s="46" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B103" s="46" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B104" s="46" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B105" s="46" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B106" s="46" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B107" s="46" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B108" s="46" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B109" s="46" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B110" s="46" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B111" s="46" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B112" s="46" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B113" s="46" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B114" s="46" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B115" s="46" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B116" s="46" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B117" s="46" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B118" s="46" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B119" s="46" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B120" s="46" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B121" s="46" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B122" s="46" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B123" s="46" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B124" s="46" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B125" s="46" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B126" s="46" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B127" s="46" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B128" s="46" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B129" s="46" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B130" s="46" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B131" s="46" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B132" s="46" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B133" s="46" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B134" s="46" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B135" s="46" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B136" s="46" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B137" s="46" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B138" s="46" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B139" s="46" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B140" s="46" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B141" s="46" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B142" s="46" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B143" s="46" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B144" s="46" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B145" s="46" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B146" s="46" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B147" s="46" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B148" s="46" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B149" s="46" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B150" s="46" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B151" s="46" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B152" s="46" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B153" s="46" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B154" s="46" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B155" s="46" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B156" s="46" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B157" s="46" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B158" s="46" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B159" s="46" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B160" s="46" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B161" s="46" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B162" s="46" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B163" s="46" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B164" s="46" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B165" s="46" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B166" s="46" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B167" s="46" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B168" s="46" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B169" s="46" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B170" s="46" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B171" s="46" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B172" s="46" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B173" s="46" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B174" s="46" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B175" s="46" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B176" s="46" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B177" s="46" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B178" s="46" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B179" s="46" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B180" s="46" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B181" s="46" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B182" s="46" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B183" s="46" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B184" s="46" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B185" s="46" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B186" s="46" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B187" s="46" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B188" s="46" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B189" s="46" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="190" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B190" s="46" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B191" s="46" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
     </row>
     <row r="192" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B192" s="46" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
     </row>
     <row r="193" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B193" s="46" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
     </row>
     <row r="194" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B194" s="46" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row r="195" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B195" s="46" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="196" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B196" s="46" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
     <row r="197" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B197" s="46" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B198" s="46" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="199" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B199" s="46" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B200" s="46" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="201" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B201" s="46" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="202" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B202" s="46" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
     <row r="203" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B203" s="46" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="204" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B204" s="46" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="205" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B205" s="46" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
     <row r="206" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B206" s="46" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="207" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B207" s="46" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row r="208" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B208" s="46" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="209" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B209" s="46" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="210" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B210" s="46" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="211" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B211" s="46" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="212" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B212" s="46" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="213" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B213" s="46" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="214" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B214" s="46" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="215" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B215" s="46" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="216" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B216" s="46" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
     </row>
     <row r="217" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B217" s="46" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row r="218" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B218" s="46" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
     </row>
     <row r="219" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B219" s="46" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
     </row>
     <row r="220" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B220" s="46" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
     </row>
     <row r="221" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B221" s="46" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
     </row>
     <row r="222" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B222" s="46" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
     </row>
     <row r="223" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B223" s="46" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
     </row>
     <row r="224" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B224" s="46" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
     </row>
     <row r="225" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B225" s="46" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
     </row>
     <row r="226" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B226" s="46" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
     </row>
     <row r="227" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B227" s="46" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="228" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B228" s="46" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
     </row>
     <row r="229" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B229" s="46" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
     </row>
     <row r="230" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B230" s="46" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
     </row>
     <row r="231" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B231" s="46" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="232" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B232" s="46" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
     </row>
     <row r="233" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B233" s="46" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
     </row>
     <row r="234" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B234" s="46" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
     </row>
     <row r="235" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B235" s="46" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
     </row>
     <row r="236" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B236" s="46" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
     </row>
     <row r="237" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B237" s="46" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
     </row>
     <row r="238" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B238" s="46" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
     </row>
     <row r="239" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B239" s="46" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
     </row>
     <row r="240" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B240" s="46" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
     </row>
     <row r="241" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B241" s="46" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
     </row>
     <row r="242" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B242" s="46" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
     </row>
     <row r="243" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B243" s="46" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
     </row>
     <row r="244" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B244" s="46" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
     </row>
     <row r="245" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B245" s="46" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
     </row>
     <row r="246" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B246" s="46" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
     </row>
     <row r="247" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B247" s="46" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
     </row>
     <row r="248" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B248" s="46" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
     </row>
     <row r="249" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B249" s="46" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
     </row>
     <row r="250" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B250" s="46" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
     </row>
     <row r="251" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B251" s="46" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
     </row>
     <row r="252" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B252" s="46" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row r="253" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B253" s="46" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
     </row>
     <row r="254" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B254" s="46" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
     </row>
     <row r="255" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B255" s="46" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
     </row>
     <row r="256" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B256" s="46" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
     </row>
     <row r="257" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B257" s="46" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
     </row>
     <row r="258" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B258" s="46" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
     </row>
     <row r="259" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B259" s="46" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
     </row>
     <row r="260" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B260" s="46" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
     </row>
     <row r="261" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B261" s="46" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
     </row>
     <row r="262" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B262" s="46" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
     </row>
     <row r="263" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B263" s="46" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
     </row>
     <row r="264" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B264" s="46" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
     </row>
     <row r="265" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B265" s="46" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
     </row>
     <row r="266" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B266" s="46" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
     </row>
     <row r="267" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B267" s="46" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
     </row>
     <row r="268" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B268" s="46" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
     </row>
     <row r="269" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B269" s="46" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
     </row>
     <row r="270" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B270" s="46" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
     </row>
     <row r="271" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B271" s="46" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
     </row>
     <row r="272" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B272" s="46" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
     </row>
     <row r="273" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B273" s="46" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
     </row>
     <row r="274" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B274" s="46" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
     </row>
     <row r="275" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B275" s="46" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
     </row>
     <row r="276" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B276" s="46" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
     </row>
     <row r="277" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B277" s="46" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
     </row>
     <row r="278" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B278" s="46" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
     </row>
     <row r="279" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B279" s="46" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="280" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B280" s="46" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
     </row>
     <row r="281" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B281" s="46" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
     </row>
     <row r="282" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B282" s="46" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
     </row>
     <row r="283" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B283" s="46" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="284" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B284" s="46" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
     </row>
     <row r="285" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B285" s="46" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
     </row>
     <row r="286" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B286" s="46" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
     </row>
     <row r="287" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B287" s="46" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
     </row>
     <row r="288" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B288" s="46" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
     </row>
     <row r="289" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B289" s="46" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
     </row>
     <row r="290" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B290" s="46" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
     </row>
     <row r="291" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B291" s="46" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
     </row>
     <row r="292" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B292" s="46" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
     </row>
     <row r="293" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B293" s="46" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
     </row>
     <row r="294" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B294" s="46" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
     </row>
     <row r="295" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B295" s="46" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
     </row>
     <row r="296" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B296" s="46" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
     </row>
     <row r="297" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B297" s="46" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
     </row>
     <row r="298" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B298" s="46" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
     </row>
     <row r="299" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B299" s="46" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
     </row>
     <row r="300" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B300" s="46" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
     </row>
     <row r="301" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B301" s="46" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
     </row>
     <row r="302" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B302" s="46" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
     </row>
     <row r="303" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B303" s="46" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
     </row>
     <row r="304" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B304" s="46" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
     </row>
     <row r="305" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B305" s="46" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
     </row>
     <row r="306" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B306" s="46" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
     </row>
     <row r="307" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B307" s="46" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
     </row>
     <row r="308" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B308" s="46" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
     </row>
     <row r="309" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B309" s="46" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
     </row>
     <row r="310" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B310" s="46" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
     </row>
     <row r="311" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B311" s="46" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
     </row>
     <row r="312" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B312" s="46" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
     </row>
     <row r="313" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B313" s="46" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
     </row>
     <row r="314" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B314" s="46" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
     </row>
     <row r="315" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B315" s="46" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
     </row>
     <row r="316" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B316" s="46" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
     </row>
     <row r="317" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B317" s="46" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
     </row>
     <row r="318" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B318" s="46" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
     </row>
     <row r="319" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B319" s="46" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="320" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B320" s="46" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
     </row>
     <row r="321" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B321" s="46" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
     </row>
     <row r="322" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B322" s="46" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
     </row>
     <row r="323" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B323" s="46" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
     </row>
     <row r="324" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B324" s="46" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
     </row>
     <row r="325" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B325" s="46" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
     </row>
     <row r="326" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B326" s="46" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
     </row>
     <row r="327" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B327" s="46" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
     </row>
     <row r="328" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B328" s="46" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
     </row>
     <row r="329" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B329" s="46" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
     </row>
     <row r="330" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B330" s="46" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
     </row>
     <row r="331" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B331" s="46" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="332" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B332" s="46" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
     </row>
     <row r="333" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B333" s="46" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
     </row>
     <row r="334" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B334" s="46" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
     </row>
     <row r="335" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B335" s="46" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
     </row>
     <row r="336" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B336" s="46" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
     </row>
     <row r="337" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B337" s="46" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
     </row>
     <row r="338" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B338" s="46" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
     </row>
     <row r="339" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B339" s="46" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
     </row>
     <row r="340" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B340" s="46" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
     </row>
     <row r="341" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B341" s="46" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
     </row>
     <row r="342" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B342" s="46" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
     </row>
     <row r="343" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B343" s="46" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
     </row>
     <row r="344" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B344" s="46" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
     </row>
     <row r="345" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B345" s="46" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
     </row>
     <row r="346" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B346" s="46" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
     </row>
     <row r="347" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B347" s="46" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
     </row>
     <row r="348" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B348" s="46" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
     </row>
     <row r="349" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B349" s="46" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
     </row>
     <row r="350" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B350" s="46" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
     </row>
     <row r="351" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B351" s="46" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
     </row>
     <row r="352" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B352" s="46" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
     </row>
     <row r="353" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B353" s="46" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
     </row>
     <row r="354" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B354" s="46" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
     </row>
     <row r="355" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B355" s="46" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="356" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B356" s="46" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
     </row>
     <row r="357" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B357" s="46" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
     </row>
     <row r="358" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B358" s="46" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
     </row>
     <row r="359" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B359" s="46" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
     </row>
     <row r="360" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B360" s="46" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
     </row>
     <row r="361" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B361" s="46" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
     </row>
     <row r="362" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B362" s="46" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
     </row>
     <row r="363" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B363" s="46" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
     </row>
     <row r="364" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B364" s="46" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
     </row>
     <row r="365" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B365" s="46" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
     </row>
     <row r="366" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B366" s="46" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
     </row>
     <row r="367" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B367" s="46" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
     </row>
     <row r="368" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B368" s="46" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
     </row>
     <row r="369" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B369" s="46" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
     </row>
     <row r="370" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B370" s="46" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
     </row>
     <row r="371" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B371" s="46" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
     </row>
     <row r="372" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B372" s="46" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
     </row>
     <row r="373" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B373" s="46" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
     </row>
     <row r="374" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B374" s="46" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
     </row>
     <row r="375" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B375" s="46" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
     </row>
     <row r="376" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B376" s="46" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
     </row>
     <row r="377" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B377" s="46" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
     </row>
     <row r="378" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B378" s="46" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
     </row>
     <row r="379" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B379" s="46" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
     </row>
     <row r="380" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B380" s="46" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
     </row>
     <row r="381" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B381" s="46" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
     </row>
     <row r="382" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B382" s="46" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
     </row>
     <row r="383" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B383" s="46" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
     </row>
     <row r="384" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B384" s="46" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
     </row>
     <row r="385" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B385" s="46" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
     </row>
     <row r="386" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>